<commit_message>
CIERRE 7 SEP 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  HERRADURA  Julio    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  HERRADURA  Julio    2023.xlsx
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="389">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1606,6 +1606,24 @@
   </si>
   <si>
     <t>NOMINA # 27</t>
+  </si>
+  <si>
+    <t>NOMINA # 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHORIZO  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONGANIZA  </t>
+  </si>
+  <si>
+    <t>COMPRAS CENTRAL--chorizo</t>
+  </si>
+  <si>
+    <t>NOMINA # 29</t>
+  </si>
+  <si>
+    <t>DEBE $ 8.00</t>
   </si>
 </sst>
 </file>
@@ -3039,7 +3057,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="386">
+  <cellXfs count="387">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3683,6 +3701,72 @@
     <xf numFmtId="16" fontId="22" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="4" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="4" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3734,69 +3818,6 @@
     <xf numFmtId="167" fontId="14" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="4" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="4" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="10" fillId="3" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3827,12 +3848,6 @@
     <xf numFmtId="166" fontId="3" fillId="7" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="51" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="51" fillId="9" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="14" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3841,6 +3856,12 @@
     </xf>
     <xf numFmtId="166" fontId="16" fillId="9" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="51" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="51" fillId="9" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="51" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -7154,23 +7175,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="348"/>
-      <c r="C1" s="350" t="s">
+      <c r="B1" s="344"/>
+      <c r="C1" s="346" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
-      <c r="G1" s="351"/>
-      <c r="H1" s="351"/>
-      <c r="I1" s="351"/>
-      <c r="J1" s="351"/>
-      <c r="K1" s="351"/>
-      <c r="L1" s="351"/>
-      <c r="M1" s="351"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
+      <c r="J1" s="347"/>
+      <c r="K1" s="347"/>
+      <c r="L1" s="347"/>
+      <c r="M1" s="347"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="349"/>
+      <c r="B2" s="345"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -7180,21 +7201,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="353"/>
+      <c r="B3" s="348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="349"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="354"/>
+      <c r="I3" s="350"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="331" t="s">
+      <c r="R3" s="353" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7209,14 +7230,14 @@
       <c r="D4" s="17">
         <v>44934</v>
       </c>
-      <c r="E4" s="333" t="s">
+      <c r="E4" s="355" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="334"/>
-      <c r="H4" s="335" t="s">
+      <c r="F4" s="356"/>
+      <c r="H4" s="357" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="336"/>
+      <c r="I4" s="358"/>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
@@ -7226,11 +7247,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="337" t="s">
+      <c r="P4" s="359" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="338"/>
-      <c r="R4" s="332"/>
+      <c r="Q4" s="360"/>
+      <c r="R4" s="354"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -9035,11 +9056,11 @@
       <c r="L49" s="76">
         <v>549</v>
       </c>
-      <c r="M49" s="355">
+      <c r="M49" s="351">
         <f>SUM(M5:M39)</f>
         <v>1666347.5</v>
       </c>
-      <c r="N49" s="340">
+      <c r="N49" s="362">
         <f>SUM(N5:N39)</f>
         <v>49399</v>
       </c>
@@ -9074,8 +9095,8 @@
       <c r="L50" s="76">
         <v>2591.1799999999998</v>
       </c>
-      <c r="M50" s="356"/>
-      <c r="N50" s="341"/>
+      <c r="M50" s="352"/>
+      <c r="N50" s="363"/>
       <c r="P50" s="36"/>
       <c r="Q50" s="9"/>
       <c r="R50" s="13">
@@ -9167,29 +9188,29 @@
       <c r="A55" s="133"/>
       <c r="B55" s="134"/>
       <c r="C55" s="1"/>
-      <c r="H55" s="342" t="s">
+      <c r="H55" s="364" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="343"/>
+      <c r="I55" s="365"/>
       <c r="J55" s="135"/>
-      <c r="K55" s="344">
+      <c r="K55" s="366">
         <f>I53+L53</f>
         <v>63475.360000000001</v>
       </c>
-      <c r="L55" s="345"/>
-      <c r="M55" s="346">
+      <c r="L55" s="367"/>
+      <c r="M55" s="368">
         <f>N49+M49</f>
         <v>1715746.5</v>
       </c>
-      <c r="N55" s="347"/>
+      <c r="N55" s="369"/>
       <c r="P55" s="36"/>
       <c r="Q55" s="9"/>
     </row>
     <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D56" s="339" t="s">
+      <c r="D56" s="361" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="339"/>
+      <c r="E56" s="361"/>
       <c r="F56" s="136">
         <f>F53-K55-C53</f>
         <v>1656897.64</v>
@@ -9200,22 +9221,22 @@
       <c r="Q56" s="9"/>
     </row>
     <row r="57" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D57" s="357" t="s">
+      <c r="D57" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="E57" s="357"/>
+      <c r="E57" s="332"/>
       <c r="F57" s="131">
         <v>-1524395.48</v>
       </c>
-      <c r="I57" s="358" t="s">
+      <c r="I57" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="J57" s="359"/>
-      <c r="K57" s="360">
+      <c r="J57" s="334"/>
+      <c r="K57" s="335">
         <f>F59+F60+F61</f>
         <v>393764.05999999994</v>
       </c>
-      <c r="L57" s="361"/>
+      <c r="L57" s="336"/>
       <c r="P57" s="36"/>
       <c r="Q57" s="9"/>
     </row>
@@ -9246,11 +9267,11 @@
         <v>18</v>
       </c>
       <c r="J59" s="147"/>
-      <c r="K59" s="362">
+      <c r="K59" s="337">
         <f>-C4</f>
         <v>-373948.72</v>
       </c>
-      <c r="L59" s="363"/>
+      <c r="L59" s="338"/>
     </row>
     <row r="60" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="148" t="s">
@@ -9267,22 +9288,22 @@
       <c r="C61" s="150">
         <v>44955</v>
       </c>
-      <c r="D61" s="364" t="s">
+      <c r="D61" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="E61" s="365"/>
+      <c r="E61" s="340"/>
       <c r="F61" s="151">
         <v>223528.9</v>
       </c>
-      <c r="I61" s="366" t="s">
+      <c r="I61" s="341" t="s">
         <v>22</v>
       </c>
-      <c r="J61" s="367"/>
-      <c r="K61" s="368">
+      <c r="J61" s="342"/>
+      <c r="K61" s="343">
         <f>K57+K59</f>
         <v>19815.339999999967</v>
       </c>
-      <c r="L61" s="368"/>
+      <c r="L61" s="343"/>
     </row>
     <row r="62" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C62" s="152"/>
@@ -9407,18 +9428,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M49:M50"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -9428,6 +9437,18 @@
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="M55:N55"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="K61:L61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10857,23 +10878,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="348"/>
-      <c r="C1" s="350" t="s">
+      <c r="B1" s="344"/>
+      <c r="C1" s="346" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
-      <c r="G1" s="351"/>
-      <c r="H1" s="351"/>
-      <c r="I1" s="351"/>
-      <c r="J1" s="351"/>
-      <c r="K1" s="351"/>
-      <c r="L1" s="351"/>
-      <c r="M1" s="351"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
+      <c r="J1" s="347"/>
+      <c r="K1" s="347"/>
+      <c r="L1" s="347"/>
+      <c r="M1" s="347"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="349"/>
+      <c r="B2" s="345"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -10886,21 +10907,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="353"/>
+      <c r="B3" s="348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="349"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="354"/>
+      <c r="I3" s="350"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="384" t="s">
+      <c r="R3" s="385" t="s">
         <v>2</v>
       </c>
     </row>
@@ -10915,14 +10936,14 @@
       <c r="D4" s="307">
         <v>45081</v>
       </c>
-      <c r="E4" s="333" t="s">
+      <c r="E4" s="355" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="334"/>
-      <c r="H4" s="335" t="s">
+      <c r="F4" s="356"/>
+      <c r="H4" s="357" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="336"/>
+      <c r="I4" s="358"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -10932,11 +10953,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="370" t="s">
+      <c r="P4" s="371" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="371"/>
-      <c r="R4" s="385"/>
+      <c r="Q4" s="372"/>
+      <c r="R4" s="386"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -12720,11 +12741,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="355">
+      <c r="M45" s="351">
         <f>SUM(M5:M39)</f>
         <v>3170751</v>
       </c>
-      <c r="N45" s="340">
+      <c r="N45" s="362">
         <f>SUM(N5:N39)</f>
         <v>31751.230000000003</v>
       </c>
@@ -12754,8 +12775,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="356"/>
-      <c r="N46" s="341"/>
+      <c r="M46" s="352"/>
+      <c r="N46" s="363"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -12847,29 +12868,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="342" t="s">
+      <c r="H51" s="364" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="343"/>
+      <c r="I51" s="365"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="344">
+      <c r="K51" s="366">
         <f>I49+L49</f>
         <v>66093.360000000015</v>
       </c>
-      <c r="L51" s="345"/>
-      <c r="M51" s="346">
+      <c r="L51" s="367"/>
+      <c r="M51" s="368">
         <f>N45+M45</f>
         <v>3202502.23</v>
       </c>
-      <c r="N51" s="347"/>
+      <c r="N51" s="369"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="339" t="s">
+      <c r="D52" s="361" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="339"/>
+      <c r="E52" s="361"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>3132761.64</v>
@@ -12880,22 +12901,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="332"/>
       <c r="F53" s="131">
         <v>-3128572.23</v>
       </c>
-      <c r="I53" s="358" t="s">
+      <c r="I53" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="359"/>
-      <c r="K53" s="372">
+      <c r="J53" s="334"/>
+      <c r="K53" s="373">
         <f>F55+F56+F57</f>
         <v>417897.52000000014</v>
       </c>
-      <c r="L53" s="373"/>
+      <c r="L53" s="374"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -12926,11 +12947,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="374">
+      <c r="K55" s="375">
         <f>-C4</f>
         <v>-345633.69</v>
       </c>
-      <c r="L55" s="375"/>
+      <c r="L55" s="376"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -12947,22 +12968,22 @@
       <c r="C57" s="150">
         <v>45109</v>
       </c>
-      <c r="D57" s="364" t="s">
+      <c r="D57" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="365"/>
+      <c r="E57" s="340"/>
       <c r="F57" s="316">
         <v>359108.11</v>
       </c>
-      <c r="I57" s="381" t="s">
+      <c r="I57" s="380" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="382"/>
-      <c r="K57" s="383">
+      <c r="J57" s="381"/>
+      <c r="K57" s="382">
         <f>K53+K55</f>
         <v>72263.830000000133</v>
       </c>
-      <c r="L57" s="383"/>
+      <c r="L57" s="382"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -13087,6 +13108,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -13096,18 +13129,6 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14492,8 +14513,8 @@
   </sheetPr>
   <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14518,23 +14539,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="348"/>
-      <c r="C1" s="350" t="s">
+      <c r="B1" s="344"/>
+      <c r="C1" s="346" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
-      <c r="G1" s="351"/>
-      <c r="H1" s="351"/>
-      <c r="I1" s="351"/>
-      <c r="J1" s="351"/>
-      <c r="K1" s="351"/>
-      <c r="L1" s="351"/>
-      <c r="M1" s="351"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
+      <c r="J1" s="347"/>
+      <c r="K1" s="347"/>
+      <c r="L1" s="347"/>
+      <c r="M1" s="347"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="349"/>
+      <c r="B2" s="345"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -14547,21 +14568,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="353"/>
+      <c r="B3" s="348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="349"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="354"/>
+      <c r="I3" s="350"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="384" t="s">
+      <c r="R3" s="385" t="s">
         <v>2</v>
       </c>
     </row>
@@ -14576,14 +14597,14 @@
       <c r="D4" s="307">
         <v>45109</v>
       </c>
-      <c r="E4" s="333" t="s">
+      <c r="E4" s="355" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="334"/>
-      <c r="H4" s="335" t="s">
+      <c r="F4" s="356"/>
+      <c r="H4" s="357" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="336"/>
+      <c r="I4" s="358"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -14593,11 +14614,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="370" t="s">
+      <c r="P4" s="371" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="371"/>
-      <c r="R4" s="385"/>
+      <c r="Q4" s="372"/>
+      <c r="R4" s="386"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -14985,35 +15006,42 @@
         <v>45118</v>
       </c>
       <c r="C13" s="25">
-        <v>0</v>
-      </c>
-      <c r="D13" s="42"/>
+        <v>3480</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>211</v>
+      </c>
       <c r="E13" s="27">
         <v>45118</v>
       </c>
-      <c r="F13" s="28"/>
+      <c r="F13" s="28">
+        <v>136861</v>
+      </c>
       <c r="G13" s="29"/>
       <c r="H13" s="30">
         <v>45118</v>
       </c>
-      <c r="I13" s="31"/>
+      <c r="I13" s="31">
+        <v>70</v>
+      </c>
       <c r="J13" s="258"/>
       <c r="K13" s="71"/>
       <c r="L13" s="259"/>
       <c r="M13" s="33">
-        <v>0</v>
+        <f>51000+81929</f>
+        <v>132929</v>
       </c>
       <c r="N13" s="34">
-        <v>0</v>
+        <v>394</v>
       </c>
       <c r="O13" s="35"/>
       <c r="P13" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>136873</v>
       </c>
       <c r="Q13" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R13" s="238">
         <v>0</v>
@@ -15026,23 +15054,29 @@
         <v>45119</v>
       </c>
       <c r="C14" s="25">
-        <v>0</v>
-      </c>
-      <c r="D14" s="46"/>
+        <v>900</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>294</v>
+      </c>
       <c r="E14" s="27">
         <v>45119</v>
       </c>
-      <c r="F14" s="28"/>
+      <c r="F14" s="28">
+        <v>28904</v>
+      </c>
       <c r="G14" s="29"/>
       <c r="H14" s="30">
         <v>45119</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="31">
+        <v>193</v>
+      </c>
       <c r="J14" s="258"/>
       <c r="K14" s="260"/>
       <c r="L14" s="259"/>
       <c r="M14" s="33">
-        <v>0</v>
+        <v>27811</v>
       </c>
       <c r="N14" s="34">
         <v>0</v>
@@ -15050,7 +15084,7 @@
       <c r="O14" s="35"/>
       <c r="P14" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28904</v>
       </c>
       <c r="Q14" s="236">
         <f t="shared" si="1"/>
@@ -15073,29 +15107,34 @@
       <c r="E15" s="27">
         <v>45120</v>
       </c>
-      <c r="F15" s="28"/>
+      <c r="F15" s="28">
+        <v>147109</v>
+      </c>
       <c r="G15" s="29"/>
       <c r="H15" s="30">
         <v>45120</v>
       </c>
-      <c r="I15" s="31"/>
+      <c r="I15" s="31">
+        <v>0</v>
+      </c>
       <c r="J15" s="258"/>
       <c r="K15" s="260"/>
       <c r="L15" s="259"/>
       <c r="M15" s="33">
-        <v>0</v>
+        <f>29000+116085</f>
+        <v>145085</v>
       </c>
       <c r="N15" s="34">
-        <v>0</v>
+        <v>2086</v>
       </c>
       <c r="O15" s="314"/>
       <c r="P15" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>147171</v>
       </c>
       <c r="Q15" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="R15" s="238">
         <v>0</v>
@@ -15108,35 +15147,42 @@
         <v>45121</v>
       </c>
       <c r="C16" s="25">
-        <v>0</v>
-      </c>
-      <c r="D16" s="52"/>
+        <v>11732</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>69</v>
+      </c>
       <c r="E16" s="27">
         <v>45121</v>
       </c>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>177601</v>
+      </c>
       <c r="G16" s="29"/>
       <c r="H16" s="30">
         <v>45121</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="31">
+        <v>158</v>
+      </c>
       <c r="J16" s="258"/>
       <c r="K16" s="260"/>
       <c r="L16" s="13"/>
       <c r="M16" s="33">
-        <v>0</v>
+        <f>57500+106095</f>
+        <v>163595</v>
       </c>
       <c r="N16" s="34">
-        <v>0</v>
+        <v>2180</v>
       </c>
       <c r="O16" s="35"/>
       <c r="P16" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>177665</v>
       </c>
       <c r="Q16" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="R16" s="238">
         <v>0</v>
@@ -15155,29 +15201,40 @@
       <c r="E17" s="27">
         <v>45122</v>
       </c>
-      <c r="F17" s="28"/>
+      <c r="F17" s="28">
+        <v>169447</v>
+      </c>
       <c r="G17" s="29"/>
       <c r="H17" s="30">
         <v>45122</v>
       </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="258"/>
-      <c r="K17" s="326"/>
-      <c r="L17" s="263"/>
+      <c r="I17" s="31">
+        <v>198</v>
+      </c>
+      <c r="J17" s="258">
+        <v>45122</v>
+      </c>
+      <c r="K17" s="45" t="s">
+        <v>383</v>
+      </c>
+      <c r="L17" s="263">
+        <v>8733</v>
+      </c>
       <c r="M17" s="33">
-        <v>0</v>
+        <f>64500+95113</f>
+        <v>159613</v>
       </c>
       <c r="N17" s="34">
-        <v>0</v>
+        <v>931</v>
       </c>
       <c r="O17" s="35"/>
       <c r="P17" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>169475</v>
       </c>
       <c r="Q17" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="R17" s="238">
         <v>0</v>
@@ -15190,35 +15247,42 @@
         <v>45123</v>
       </c>
       <c r="C18" s="25">
-        <v>0</v>
-      </c>
-      <c r="D18" s="38"/>
+        <v>1980</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>384</v>
+      </c>
       <c r="E18" s="27">
         <v>45123</v>
       </c>
-      <c r="F18" s="28"/>
+      <c r="F18" s="28">
+        <v>144827</v>
+      </c>
       <c r="G18" s="29"/>
       <c r="H18" s="30">
         <v>45123</v>
       </c>
-      <c r="I18" s="31"/>
+      <c r="I18" s="31">
+        <v>15</v>
+      </c>
       <c r="J18" s="258"/>
       <c r="K18" s="265"/>
       <c r="L18" s="259"/>
       <c r="M18" s="33">
-        <v>0</v>
+        <f>128100+14367</f>
+        <v>142467</v>
       </c>
       <c r="N18" s="34">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="O18" s="35"/>
       <c r="P18" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>144838</v>
       </c>
       <c r="Q18" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="R18" s="238">
         <v>0</v>
@@ -15237,17 +15301,22 @@
       <c r="E19" s="27">
         <v>45124</v>
       </c>
-      <c r="F19" s="28"/>
+      <c r="F19" s="28">
+        <v>174056</v>
+      </c>
       <c r="G19" s="29"/>
       <c r="H19" s="30">
         <v>45124</v>
       </c>
-      <c r="I19" s="31"/>
+      <c r="I19" s="31">
+        <v>234</v>
+      </c>
       <c r="J19" s="258"/>
       <c r="K19" s="266"/>
       <c r="L19" s="267"/>
       <c r="M19" s="33">
-        <v>0</v>
+        <f>35800+138022</f>
+        <v>173822</v>
       </c>
       <c r="N19" s="34">
         <v>0</v>
@@ -15255,7 +15324,7 @@
       <c r="O19" s="35"/>
       <c r="P19" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>174056</v>
       </c>
       <c r="Q19" s="236">
         <f t="shared" si="1"/>
@@ -15278,29 +15347,34 @@
       <c r="E20" s="27">
         <v>45125</v>
       </c>
-      <c r="F20" s="28"/>
+      <c r="F20" s="28">
+        <v>154400</v>
+      </c>
       <c r="G20" s="29"/>
       <c r="H20" s="30">
         <v>45125</v>
       </c>
-      <c r="I20" s="31"/>
+      <c r="I20" s="31">
+        <v>47</v>
+      </c>
       <c r="J20" s="258"/>
       <c r="K20" s="262"/>
       <c r="L20" s="263"/>
       <c r="M20" s="33">
-        <v>0</v>
+        <f>82600+71397</f>
+        <v>153997</v>
       </c>
       <c r="N20" s="34">
-        <v>0</v>
+        <v>367</v>
       </c>
       <c r="O20" s="35"/>
       <c r="P20" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>154411</v>
       </c>
       <c r="Q20" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="R20" s="238">
         <v>0</v>
@@ -15319,17 +15393,22 @@
       <c r="E21" s="27">
         <v>45126</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="28">
+        <v>86346</v>
+      </c>
       <c r="G21" s="29"/>
       <c r="H21" s="30">
         <v>45126</v>
       </c>
-      <c r="I21" s="31"/>
+      <c r="I21" s="31">
+        <v>159</v>
+      </c>
       <c r="J21" s="258"/>
       <c r="K21" s="268"/>
       <c r="L21" s="263"/>
       <c r="M21" s="33">
-        <v>0</v>
+        <f>72187+14000</f>
+        <v>86187</v>
       </c>
       <c r="N21" s="34">
         <v>0</v>
@@ -15337,7 +15416,7 @@
       <c r="O21" s="35"/>
       <c r="P21" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>86346</v>
       </c>
       <c r="Q21" s="236">
         <f t="shared" si="1"/>
@@ -15354,35 +15433,42 @@
         <v>45127</v>
       </c>
       <c r="C22" s="25">
-        <v>0</v>
-      </c>
-      <c r="D22" s="46"/>
+        <v>3000</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>385</v>
+      </c>
       <c r="E22" s="27">
         <v>45127</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="28">
+        <v>155372</v>
+      </c>
       <c r="G22" s="29"/>
       <c r="H22" s="30">
         <v>45127</v>
       </c>
-      <c r="I22" s="31"/>
+      <c r="I22" s="31">
+        <v>15</v>
+      </c>
       <c r="J22" s="258"/>
       <c r="K22" s="302"/>
       <c r="L22" s="269"/>
       <c r="M22" s="33">
-        <v>0</v>
+        <f>137720+14000</f>
+        <v>151720</v>
       </c>
       <c r="N22" s="34">
-        <v>0</v>
+        <v>657</v>
       </c>
       <c r="O22" s="315"/>
       <c r="P22" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>155392</v>
       </c>
       <c r="Q22" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R22" s="238">
         <v>0</v>
@@ -15395,35 +15481,42 @@
         <v>45128</v>
       </c>
       <c r="C23" s="25">
-        <v>0</v>
-      </c>
-      <c r="D23" s="46"/>
+        <v>29665</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>386</v>
+      </c>
       <c r="E23" s="27">
         <v>45128</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="28">
+        <v>152771</v>
+      </c>
       <c r="G23" s="29"/>
       <c r="H23" s="30">
         <v>45128</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="31">
+        <v>160</v>
+      </c>
       <c r="J23" s="270"/>
       <c r="K23" s="271"/>
       <c r="L23" s="263"/>
       <c r="M23" s="33">
-        <v>0</v>
+        <f>11000+110343</f>
+        <v>121343</v>
       </c>
       <c r="N23" s="34">
-        <v>0</v>
+        <v>1650</v>
       </c>
       <c r="O23" s="35"/>
       <c r="P23" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>152818</v>
       </c>
       <c r="Q23" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="R23" s="238">
         <v>0</v>
@@ -15442,29 +15535,42 @@
       <c r="E24" s="27">
         <v>45129</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="28">
+        <v>161197</v>
+      </c>
       <c r="G24" s="29"/>
       <c r="H24" s="30">
         <v>45129</v>
       </c>
-      <c r="I24" s="31"/>
-      <c r="J24" s="272"/>
-      <c r="K24" s="271"/>
-      <c r="L24" s="273"/>
+      <c r="I24" s="31">
+        <v>114</v>
+      </c>
+      <c r="J24" s="272">
+        <v>45129</v>
+      </c>
+      <c r="K24" s="271" t="s">
+        <v>387</v>
+      </c>
+      <c r="L24" s="273">
+        <v>9554</v>
+      </c>
       <c r="M24" s="33">
-        <v>0</v>
+        <f>104500+45910</f>
+        <v>150410</v>
       </c>
       <c r="N24" s="34">
-        <v>0</v>
-      </c>
-      <c r="O24" s="35"/>
+        <v>1145</v>
+      </c>
+      <c r="O24" s="331" t="s">
+        <v>388</v>
+      </c>
       <c r="P24" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>161223</v>
       </c>
       <c r="Q24" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="R24" s="238">
         <v>0</v>
@@ -15483,29 +15589,34 @@
       <c r="E25" s="27">
         <v>45130</v>
       </c>
-      <c r="F25" s="28"/>
+      <c r="F25" s="28">
+        <v>137636</v>
+      </c>
       <c r="G25" s="29"/>
       <c r="H25" s="30">
         <v>45130</v>
       </c>
-      <c r="I25" s="31"/>
+      <c r="I25" s="31">
+        <v>5</v>
+      </c>
       <c r="J25" s="274"/>
       <c r="K25" s="275"/>
       <c r="L25" s="276"/>
       <c r="M25" s="33">
-        <v>0</v>
+        <f>123800+12948</f>
+        <v>136748</v>
       </c>
       <c r="N25" s="34">
-        <v>0</v>
+        <v>910</v>
       </c>
       <c r="O25" s="35"/>
       <c r="P25" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>137663</v>
       </c>
       <c r="Q25" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R25" s="238">
         <v>0</v>
@@ -16200,21 +16311,21 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="355">
+      <c r="M45" s="351">
         <f>SUM(M5:M39)</f>
-        <v>1030358</v>
-      </c>
-      <c r="N45" s="340">
+        <v>2776085</v>
+      </c>
+      <c r="N45" s="362">
         <f>SUM(N5:N39)</f>
-        <v>3027</v>
+        <v>13723</v>
       </c>
       <c r="P45" s="98">
         <f t="shared" si="0"/>
-        <v>1033385</v>
+        <v>2789808</v>
       </c>
       <c r="Q45" s="236">
         <f t="shared" si="1"/>
-        <v>1033385</v>
+        <v>2789808</v>
       </c>
       <c r="R45" s="329">
         <f>SUM(R5:R39)</f>
@@ -16234,8 +16345,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="356"/>
-      <c r="N46" s="341"/>
+      <c r="M46" s="352"/>
+      <c r="N46" s="363"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="236">
         <f t="shared" si="1"/>
@@ -16291,7 +16402,7 @@
       </c>
       <c r="C49" s="122">
         <f>SUM(C5:C48)</f>
-        <v>9041</v>
+        <v>59798</v>
       </c>
       <c r="D49" s="123"/>
       <c r="E49" s="124" t="s">
@@ -16299,7 +16410,7 @@
       </c>
       <c r="F49" s="125">
         <f>SUM(F5:F48)</f>
-        <v>997801</v>
+        <v>2824328</v>
       </c>
       <c r="G49" s="123"/>
       <c r="H49" s="126" t="s">
@@ -16307,7 +16418,7 @@
       </c>
       <c r="I49" s="127">
         <f>SUM(I5:I48)</f>
-        <v>987</v>
+        <v>2355</v>
       </c>
       <c r="J49" s="290"/>
       <c r="K49" s="291" t="s">
@@ -16315,7 +16426,7 @@
       </c>
       <c r="L49" s="292">
         <f>SUM(L5:L48)</f>
-        <v>9055</v>
+        <v>27342</v>
       </c>
       <c r="M49" s="131"/>
       <c r="N49" s="131"/>
@@ -16333,32 +16444,32 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="342" t="s">
+      <c r="H51" s="364" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="343"/>
+      <c r="I51" s="365"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="344">
+      <c r="K51" s="366">
         <f>I49+L49</f>
-        <v>10042</v>
-      </c>
-      <c r="L51" s="345"/>
-      <c r="M51" s="346">
+        <v>29697</v>
+      </c>
+      <c r="L51" s="367"/>
+      <c r="M51" s="368">
         <f>N45+M45</f>
-        <v>1033385</v>
-      </c>
-      <c r="N51" s="347"/>
+        <v>2789808</v>
+      </c>
+      <c r="N51" s="369"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="339" t="s">
+      <c r="D52" s="361" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="339"/>
+      <c r="E52" s="361"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
-        <v>978718</v>
+        <v>2734833</v>
       </c>
       <c r="I52" s="137"/>
       <c r="J52" s="138"/>
@@ -16366,22 +16477,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="332"/>
       <c r="F53" s="131">
         <v>0</v>
       </c>
-      <c r="I53" s="358" t="s">
+      <c r="I53" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="359"/>
-      <c r="K53" s="372">
+      <c r="J53" s="334"/>
+      <c r="K53" s="373">
         <f>F55+F56+F57</f>
-        <v>1336946.1200000001</v>
-      </c>
-      <c r="L53" s="373"/>
+        <v>3093061.12</v>
+      </c>
+      <c r="L53" s="374"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -16406,18 +16517,18 @@
       </c>
       <c r="F55" s="131">
         <f>SUM(F52:F54)</f>
-        <v>978718</v>
+        <v>2734833</v>
       </c>
       <c r="H55" s="23"/>
       <c r="I55" s="146" t="s">
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="374">
+      <c r="K55" s="375">
         <f>-C4</f>
         <v>-359108.11</v>
       </c>
-      <c r="L55" s="375"/>
+      <c r="L55" s="376"/>
       <c r="Q55" s="9"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -16435,22 +16546,22 @@
       <c r="C57" s="150">
         <v>45137</v>
       </c>
-      <c r="D57" s="364" t="s">
+      <c r="D57" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="365"/>
+      <c r="E57" s="340"/>
       <c r="F57" s="316">
         <v>358228.12</v>
       </c>
-      <c r="I57" s="381" t="s">
+      <c r="I57" s="380" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="382"/>
-      <c r="K57" s="383">
+      <c r="J57" s="381"/>
+      <c r="K57" s="382">
         <f>K53+K55</f>
-        <v>977838.01000000013</v>
-      </c>
-      <c r="L57" s="383"/>
+        <v>2733953.0100000002</v>
+      </c>
+      <c r="L57" s="382"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -16575,6 +16686,20 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="N45:N46"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="I53:J53"/>
     <mergeCell ref="K53:L53"/>
@@ -16582,20 +16707,6 @@
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="I57:J57"/>
     <mergeCell ref="K57:L57"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="N45:N46"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19064,23 +19175,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="348"/>
-      <c r="C1" s="350" t="s">
+      <c r="B1" s="344"/>
+      <c r="C1" s="346" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
-      <c r="G1" s="351"/>
-      <c r="H1" s="351"/>
-      <c r="I1" s="351"/>
-      <c r="J1" s="351"/>
-      <c r="K1" s="351"/>
-      <c r="L1" s="351"/>
-      <c r="M1" s="351"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
+      <c r="J1" s="347"/>
+      <c r="K1" s="347"/>
+      <c r="L1" s="347"/>
+      <c r="M1" s="347"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="349"/>
+      <c r="B2" s="345"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -19090,21 +19201,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="353"/>
+      <c r="B3" s="348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="349"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="354"/>
+      <c r="I3" s="350"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="331" t="s">
+      <c r="R3" s="353" t="s">
         <v>2</v>
       </c>
     </row>
@@ -19119,14 +19230,14 @@
       <c r="D4" s="17">
         <v>44955</v>
       </c>
-      <c r="E4" s="333" t="s">
+      <c r="E4" s="355" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="334"/>
-      <c r="H4" s="335" t="s">
+      <c r="F4" s="356"/>
+      <c r="H4" s="357" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="336"/>
+      <c r="I4" s="358"/>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
@@ -19136,11 +19247,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="370" t="s">
+      <c r="P4" s="371" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="371"/>
-      <c r="R4" s="369"/>
+      <c r="Q4" s="372"/>
+      <c r="R4" s="370"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -20941,11 +21052,11 @@
       <c r="J45" s="74"/>
       <c r="K45" s="97"/>
       <c r="L45" s="76"/>
-      <c r="M45" s="355">
+      <c r="M45" s="351">
         <f>SUM(M5:M39)</f>
         <v>2238523</v>
       </c>
-      <c r="N45" s="340">
+      <c r="N45" s="362">
         <f>SUM(N5:N39)</f>
         <v>97258</v>
       </c>
@@ -20975,8 +21086,8 @@
       <c r="J46" s="74"/>
       <c r="K46" s="102"/>
       <c r="L46" s="76"/>
-      <c r="M46" s="356"/>
-      <c r="N46" s="341"/>
+      <c r="M46" s="352"/>
+      <c r="N46" s="363"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -21068,29 +21179,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="342" t="s">
+      <c r="H51" s="364" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="343"/>
+      <c r="I51" s="365"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="344">
+      <c r="K51" s="366">
         <f>I49+L49</f>
         <v>90767.040000000008</v>
       </c>
-      <c r="L51" s="345"/>
-      <c r="M51" s="346">
+      <c r="L51" s="367"/>
+      <c r="M51" s="368">
         <f>N45+M45</f>
         <v>2335781</v>
       </c>
-      <c r="N51" s="347"/>
+      <c r="N51" s="369"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D52" s="339" t="s">
+      <c r="D52" s="361" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="339"/>
+      <c r="E52" s="361"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2261973.96</v>
@@ -21101,22 +21212,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="332"/>
       <c r="F53" s="131">
         <v>-2224189.7400000002</v>
       </c>
-      <c r="I53" s="358" t="s">
+      <c r="I53" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="359"/>
-      <c r="K53" s="360">
+      <c r="J53" s="334"/>
+      <c r="K53" s="335">
         <f>F55+F56+F57</f>
         <v>296963.76999999973</v>
       </c>
-      <c r="L53" s="361"/>
+      <c r="L53" s="336"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -21147,11 +21258,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="362">
+      <c r="K55" s="337">
         <f>-C4</f>
         <v>-223528.9</v>
       </c>
-      <c r="L55" s="363"/>
+      <c r="L55" s="338"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -21168,22 +21279,22 @@
       <c r="C57" s="150">
         <v>44985</v>
       </c>
-      <c r="D57" s="364" t="s">
+      <c r="D57" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="365"/>
+      <c r="E57" s="340"/>
       <c r="F57" s="151">
         <v>230554.55</v>
       </c>
-      <c r="I57" s="366" t="s">
+      <c r="I57" s="341" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="367"/>
-      <c r="K57" s="368">
+      <c r="J57" s="342"/>
+      <c r="K57" s="343">
         <f>K53+K55</f>
         <v>73434.869999999733</v>
       </c>
-      <c r="L57" s="368"/>
+      <c r="L57" s="343"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -21308,18 +21419,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -21329,6 +21428,18 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22787,23 +22898,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="348"/>
-      <c r="C1" s="350" t="s">
+      <c r="B1" s="344"/>
+      <c r="C1" s="346" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
-      <c r="G1" s="351"/>
-      <c r="H1" s="351"/>
-      <c r="I1" s="351"/>
-      <c r="J1" s="351"/>
-      <c r="K1" s="351"/>
-      <c r="L1" s="351"/>
-      <c r="M1" s="351"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
+      <c r="J1" s="347"/>
+      <c r="K1" s="347"/>
+      <c r="L1" s="347"/>
+      <c r="M1" s="347"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="349"/>
+      <c r="B2" s="345"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -22813,21 +22924,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="353"/>
+      <c r="B3" s="348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="349"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="354"/>
+      <c r="I3" s="350"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="331" t="s">
+      <c r="R3" s="353" t="s">
         <v>2</v>
       </c>
     </row>
@@ -22842,14 +22953,14 @@
       <c r="D4" s="17">
         <v>44985</v>
       </c>
-      <c r="E4" s="333" t="s">
+      <c r="E4" s="355" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="334"/>
-      <c r="H4" s="335" t="s">
+      <c r="F4" s="356"/>
+      <c r="H4" s="357" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="336"/>
+      <c r="I4" s="358"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -22859,11 +22970,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="370" t="s">
+      <c r="P4" s="371" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="371"/>
-      <c r="R4" s="369"/>
+      <c r="Q4" s="372"/>
+      <c r="R4" s="370"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -24656,11 +24767,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="231"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="355">
+      <c r="M45" s="351">
         <f>SUM(M5:M39)</f>
         <v>2689952</v>
       </c>
-      <c r="N45" s="340">
+      <c r="N45" s="362">
         <f>SUM(N5:N39)</f>
         <v>61422</v>
       </c>
@@ -24690,8 +24801,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="356"/>
-      <c r="N46" s="341"/>
+      <c r="M46" s="352"/>
+      <c r="N46" s="363"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -24783,29 +24894,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="342" t="s">
+      <c r="H51" s="364" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="343"/>
+      <c r="I51" s="365"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="344">
+      <c r="K51" s="366">
         <f>I49+L49</f>
         <v>425400.67</v>
       </c>
-      <c r="L51" s="345"/>
-      <c r="M51" s="346">
+      <c r="L51" s="367"/>
+      <c r="M51" s="368">
         <f>N45+M45</f>
         <v>2751374</v>
       </c>
-      <c r="N51" s="347"/>
+      <c r="N51" s="369"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="339" t="s">
+      <c r="D52" s="361" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="339"/>
+      <c r="E52" s="361"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2464124.33</v>
@@ -24816,22 +24927,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="332"/>
       <c r="F53" s="131">
         <v>-2869426.04</v>
       </c>
-      <c r="I53" s="358" t="s">
+      <c r="I53" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="359"/>
-      <c r="K53" s="372">
+      <c r="J53" s="334"/>
+      <c r="K53" s="373">
         <f>F55+F56+F57</f>
         <v>-32021.369999999937</v>
       </c>
-      <c r="L53" s="373"/>
+      <c r="L53" s="374"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -24862,11 +24973,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="374">
+      <c r="K55" s="375">
         <f>-C4</f>
         <v>-230554.55</v>
       </c>
-      <c r="L55" s="375"/>
+      <c r="L55" s="376"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -24883,22 +24994,22 @@
       <c r="C57" s="150">
         <v>45015</v>
       </c>
-      <c r="D57" s="364" t="s">
+      <c r="D57" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="365"/>
+      <c r="E57" s="340"/>
       <c r="F57" s="151">
         <v>341192.34</v>
       </c>
-      <c r="I57" s="376" t="s">
+      <c r="I57" s="377" t="s">
         <v>170</v>
       </c>
-      <c r="J57" s="377"/>
-      <c r="K57" s="378">
+      <c r="J57" s="378"/>
+      <c r="K57" s="379">
         <f>K53+K55</f>
         <v>-262575.91999999993</v>
       </c>
-      <c r="L57" s="378"/>
+      <c r="L57" s="379"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -25023,6 +25134,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -25032,18 +25155,6 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26445,23 +26556,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="348"/>
-      <c r="C1" s="350" t="s">
+      <c r="B1" s="344"/>
+      <c r="C1" s="346" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
-      <c r="G1" s="351"/>
-      <c r="H1" s="351"/>
-      <c r="I1" s="351"/>
-      <c r="J1" s="351"/>
-      <c r="K1" s="351"/>
-      <c r="L1" s="351"/>
-      <c r="M1" s="351"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
+      <c r="J1" s="347"/>
+      <c r="K1" s="347"/>
+      <c r="L1" s="347"/>
+      <c r="M1" s="347"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="349"/>
+      <c r="B2" s="345"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -26474,21 +26585,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="353"/>
+      <c r="B3" s="348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="349"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="354"/>
+      <c r="I3" s="350"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="379" t="s">
+      <c r="R3" s="383" t="s">
         <v>2</v>
       </c>
     </row>
@@ -26503,14 +26614,14 @@
       <c r="D4" s="17">
         <v>45015</v>
       </c>
-      <c r="E4" s="333" t="s">
+      <c r="E4" s="355" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="334"/>
-      <c r="H4" s="335" t="s">
+      <c r="F4" s="356"/>
+      <c r="H4" s="357" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="336"/>
+      <c r="I4" s="358"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -26520,11 +26631,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="370" t="s">
+      <c r="P4" s="371" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="371"/>
-      <c r="R4" s="380"/>
+      <c r="Q4" s="372"/>
+      <c r="R4" s="384"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -28411,11 +28522,11 @@
       <c r="L45" s="312">
         <v>2123.98</v>
       </c>
-      <c r="M45" s="355">
+      <c r="M45" s="351">
         <f>SUM(M5:M39)</f>
         <v>2488709</v>
       </c>
-      <c r="N45" s="340">
+      <c r="N45" s="362">
         <f>SUM(N5:N39)</f>
         <v>78710</v>
       </c>
@@ -28451,8 +28562,8 @@
       <c r="L46" s="281">
         <v>34015</v>
       </c>
-      <c r="M46" s="356"/>
-      <c r="N46" s="341"/>
+      <c r="M46" s="352"/>
+      <c r="N46" s="363"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -28544,29 +28655,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="342" t="s">
+      <c r="H51" s="364" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="343"/>
+      <c r="I51" s="365"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="344">
+      <c r="K51" s="366">
         <f>I49+L49</f>
         <v>124244.06999999999</v>
       </c>
-      <c r="L51" s="345"/>
-      <c r="M51" s="346">
+      <c r="L51" s="367"/>
+      <c r="M51" s="368">
         <f>N45+M45</f>
         <v>2567419</v>
       </c>
-      <c r="N51" s="347"/>
+      <c r="N51" s="369"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="339" t="s">
+      <c r="D52" s="361" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="339"/>
+      <c r="E52" s="361"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2480239.9300000002</v>
@@ -28577,22 +28688,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="332"/>
       <c r="F53" s="131">
         <v>-2463938.5299999998</v>
       </c>
-      <c r="I53" s="358" t="s">
+      <c r="I53" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="359"/>
-      <c r="K53" s="372">
+      <c r="J53" s="334"/>
+      <c r="K53" s="373">
         <f>F55+F56+F57</f>
         <v>439109.10000000038</v>
       </c>
-      <c r="L53" s="373"/>
+      <c r="L53" s="374"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -28623,11 +28734,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="374">
+      <c r="K55" s="375">
         <f>-C4</f>
         <v>-341192.34</v>
       </c>
-      <c r="L55" s="375"/>
+      <c r="L55" s="376"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -28644,22 +28755,22 @@
       <c r="C57" s="150">
         <v>45050</v>
       </c>
-      <c r="D57" s="364" t="s">
+      <c r="D57" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="365"/>
+      <c r="E57" s="340"/>
       <c r="F57" s="151">
         <v>394548.7</v>
       </c>
-      <c r="I57" s="381" t="s">
+      <c r="I57" s="380" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="382"/>
-      <c r="K57" s="383">
+      <c r="J57" s="381"/>
+      <c r="K57" s="382">
         <f>K53+K55</f>
         <v>97916.760000000359</v>
       </c>
-      <c r="L57" s="383"/>
+      <c r="L57" s="382"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -28784,18 +28895,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -28805,6 +28904,18 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30196,23 +30307,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="348"/>
-      <c r="C1" s="350" t="s">
+      <c r="B1" s="344"/>
+      <c r="C1" s="346" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="351"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="351"/>
-      <c r="G1" s="351"/>
-      <c r="H1" s="351"/>
-      <c r="I1" s="351"/>
-      <c r="J1" s="351"/>
-      <c r="K1" s="351"/>
-      <c r="L1" s="351"/>
-      <c r="M1" s="351"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="347"/>
+      <c r="I1" s="347"/>
+      <c r="J1" s="347"/>
+      <c r="K1" s="347"/>
+      <c r="L1" s="347"/>
+      <c r="M1" s="347"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="349"/>
+      <c r="B2" s="345"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -30225,21 +30336,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="353"/>
+      <c r="B3" s="348" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="349"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="354"/>
+      <c r="I3" s="350"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="384" t="s">
+      <c r="R3" s="385" t="s">
         <v>2</v>
       </c>
     </row>
@@ -30254,14 +30365,14 @@
       <c r="D4" s="307">
         <v>45050</v>
       </c>
-      <c r="E4" s="333" t="s">
+      <c r="E4" s="355" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="334"/>
-      <c r="H4" s="335" t="s">
+      <c r="F4" s="356"/>
+      <c r="H4" s="357" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="336"/>
+      <c r="I4" s="358"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -30271,11 +30382,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="370" t="s">
+      <c r="P4" s="371" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="371"/>
-      <c r="R4" s="385"/>
+      <c r="Q4" s="372"/>
+      <c r="R4" s="386"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -32148,11 +32259,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="355">
+      <c r="M45" s="351">
         <f>SUM(M5:M39)</f>
         <v>3007589</v>
       </c>
-      <c r="N45" s="340">
+      <c r="N45" s="362">
         <f>SUM(N5:N39)</f>
         <v>29752</v>
       </c>
@@ -32182,8 +32293,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="356"/>
-      <c r="N46" s="341"/>
+      <c r="M46" s="352"/>
+      <c r="N46" s="363"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -32275,29 +32386,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="342" t="s">
+      <c r="H51" s="364" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="343"/>
+      <c r="I51" s="365"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="344">
+      <c r="K51" s="366">
         <f>I49+L49</f>
         <v>84500.43</v>
       </c>
-      <c r="L51" s="345"/>
-      <c r="M51" s="346">
+      <c r="L51" s="367"/>
+      <c r="M51" s="368">
         <f>N45+M45</f>
         <v>3037341</v>
       </c>
-      <c r="N51" s="347"/>
+      <c r="N51" s="369"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="339" t="s">
+      <c r="D52" s="361" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="339"/>
+      <c r="E52" s="361"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2988109.57</v>
@@ -32308,22 +32419,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="332"/>
       <c r="F53" s="131">
         <v>-2955802.29</v>
       </c>
-      <c r="I53" s="358" t="s">
+      <c r="I53" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="359"/>
-      <c r="K53" s="372">
+      <c r="J53" s="334"/>
+      <c r="K53" s="373">
         <f>F55+F56+F57</f>
         <v>419364.9699999998</v>
       </c>
-      <c r="L53" s="373"/>
+      <c r="L53" s="374"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -32354,11 +32465,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="374">
+      <c r="K55" s="375">
         <f>-C4</f>
         <v>-394548.7</v>
       </c>
-      <c r="L55" s="375"/>
+      <c r="L55" s="376"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -32375,22 +32486,22 @@
       <c r="C57" s="150">
         <v>45081</v>
       </c>
-      <c r="D57" s="364" t="s">
+      <c r="D57" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="365"/>
+      <c r="E57" s="340"/>
       <c r="F57" s="316">
         <v>345633.69</v>
       </c>
-      <c r="I57" s="381" t="s">
+      <c r="I57" s="380" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="382"/>
-      <c r="K57" s="383">
+      <c r="J57" s="381"/>
+      <c r="K57" s="382">
         <f>K53+K55</f>
         <v>24816.269999999786</v>
       </c>
-      <c r="L57" s="383"/>
+      <c r="L57" s="382"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -32515,6 +32626,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -32524,18 +32647,6 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="90" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
cierre 11 SEPT 2023
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  HERRADURA  Julio    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  HERRADURA  Julio    2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20715" windowHeight="11730" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20715" windowHeight="11730" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="  E N E R O    2 0 2 3     " sheetId="1" r:id="rId1"/>
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="451">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1639,6 +1639,177 @@
   </si>
   <si>
     <t xml:space="preserve">Comision </t>
+  </si>
+  <si>
+    <t>15304 E</t>
+  </si>
+  <si>
+    <t>15348 E</t>
+  </si>
+  <si>
+    <t>15501 E</t>
+  </si>
+  <si>
+    <t>15578 E</t>
+  </si>
+  <si>
+    <t>15735 E</t>
+  </si>
+  <si>
+    <t>15751 E</t>
+  </si>
+  <si>
+    <t>15780 E</t>
+  </si>
+  <si>
+    <t>15785 E</t>
+  </si>
+  <si>
+    <t>15956 E</t>
+  </si>
+  <si>
+    <t>15825 E</t>
+  </si>
+  <si>
+    <t>16008 E</t>
+  </si>
+  <si>
+    <t>16078 E</t>
+  </si>
+  <si>
+    <t>16124 E</t>
+  </si>
+  <si>
+    <t>16182 E</t>
+  </si>
+  <si>
+    <t>16252 E</t>
+  </si>
+  <si>
+    <t>16253 E</t>
+  </si>
+  <si>
+    <t>16351 E</t>
+  </si>
+  <si>
+    <t>16502 E</t>
+  </si>
+  <si>
+    <t>16566 E</t>
+  </si>
+  <si>
+    <t>16567 E</t>
+  </si>
+  <si>
+    <t>16569 E</t>
+  </si>
+  <si>
+    <t>16654 E</t>
+  </si>
+  <si>
+    <t>16740 E</t>
+  </si>
+  <si>
+    <t>167587 E</t>
+  </si>
+  <si>
+    <t>16758 E</t>
+  </si>
+  <si>
+    <t>16831 E</t>
+  </si>
+  <si>
+    <t>16833 E</t>
+  </si>
+  <si>
+    <t>16836 E</t>
+  </si>
+  <si>
+    <t>16882 E</t>
+  </si>
+  <si>
+    <t>16986 E</t>
+  </si>
+  <si>
+    <t>16987 E</t>
+  </si>
+  <si>
+    <t>17005 E</t>
+  </si>
+  <si>
+    <t>17006 E</t>
+  </si>
+  <si>
+    <t>17079 E</t>
+  </si>
+  <si>
+    <t>17082 E</t>
+  </si>
+  <si>
+    <t>17243 E</t>
+  </si>
+  <si>
+    <t>17244 E</t>
+  </si>
+  <si>
+    <t>17245 E</t>
+  </si>
+  <si>
+    <t>17277 E</t>
+  </si>
+  <si>
+    <t>17278 E</t>
+  </si>
+  <si>
+    <t>17426 E</t>
+  </si>
+  <si>
+    <t>17427 E</t>
+  </si>
+  <si>
+    <t>17438 E</t>
+  </si>
+  <si>
+    <t>17439 E</t>
+  </si>
+  <si>
+    <t>17465 E</t>
+  </si>
+  <si>
+    <t>17516 E</t>
+  </si>
+  <si>
+    <t>17682 E</t>
+  </si>
+  <si>
+    <t>17683 E</t>
+  </si>
+  <si>
+    <t>17815 E</t>
+  </si>
+  <si>
+    <t>17822 E</t>
+  </si>
+  <si>
+    <t>17842 E</t>
+  </si>
+  <si>
+    <t>17922 E</t>
+  </si>
+  <si>
+    <t>17923 E</t>
+  </si>
+  <si>
+    <t>17951 E</t>
+  </si>
+  <si>
+    <t>18064 E</t>
+  </si>
+  <si>
+    <t>18065 E</t>
+  </si>
+  <si>
+    <t>18074 E</t>
   </si>
 </sst>
 </file>
@@ -3072,7 +3243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="388">
+  <cellXfs count="398">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3719,6 +3890,36 @@
     <xf numFmtId="16" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="37" fillId="7" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="48" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="40" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="40" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="40" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3884,8 +4085,8 @@
     <xf numFmtId="44" fontId="51" fillId="12" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="166" fontId="16" fillId="7" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7193,23 +7394,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="354"/>
+      <c r="C1" s="356" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="355"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -7219,21 +7420,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="358" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="359"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="360"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="353" t="s">
+      <c r="R3" s="363" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7248,14 +7449,14 @@
       <c r="D4" s="17">
         <v>44934</v>
       </c>
-      <c r="E4" s="355" t="s">
+      <c r="E4" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="356"/>
-      <c r="H4" s="357" t="s">
+      <c r="F4" s="366"/>
+      <c r="H4" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="358"/>
+      <c r="I4" s="368"/>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
@@ -7265,11 +7466,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="359" t="s">
+      <c r="P4" s="369" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="360"/>
-      <c r="R4" s="354"/>
+      <c r="Q4" s="370"/>
+      <c r="R4" s="364"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -9074,11 +9275,11 @@
       <c r="L49" s="76">
         <v>549</v>
       </c>
-      <c r="M49" s="351">
+      <c r="M49" s="361">
         <f>SUM(M5:M39)</f>
         <v>1666347.5</v>
       </c>
-      <c r="N49" s="362">
+      <c r="N49" s="372">
         <f>SUM(N5:N39)</f>
         <v>49399</v>
       </c>
@@ -9113,8 +9314,8 @@
       <c r="L50" s="76">
         <v>2591.1799999999998</v>
       </c>
-      <c r="M50" s="352"/>
-      <c r="N50" s="363"/>
+      <c r="M50" s="362"/>
+      <c r="N50" s="373"/>
       <c r="P50" s="36"/>
       <c r="Q50" s="9"/>
       <c r="R50" s="13">
@@ -9206,29 +9407,29 @@
       <c r="A55" s="133"/>
       <c r="B55" s="134"/>
       <c r="C55" s="1"/>
-      <c r="H55" s="364" t="s">
+      <c r="H55" s="374" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="365"/>
+      <c r="I55" s="375"/>
       <c r="J55" s="135"/>
-      <c r="K55" s="366">
+      <c r="K55" s="376">
         <f>I53+L53</f>
         <v>63475.360000000001</v>
       </c>
-      <c r="L55" s="367"/>
-      <c r="M55" s="368">
+      <c r="L55" s="377"/>
+      <c r="M55" s="378">
         <f>N49+M49</f>
         <v>1715746.5</v>
       </c>
-      <c r="N55" s="369"/>
+      <c r="N55" s="379"/>
       <c r="P55" s="36"/>
       <c r="Q55" s="9"/>
     </row>
     <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D56" s="361" t="s">
+      <c r="D56" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="361"/>
+      <c r="E56" s="371"/>
       <c r="F56" s="136">
         <f>F53-K55-C53</f>
         <v>1656897.64</v>
@@ -9239,22 +9440,22 @@
       <c r="Q56" s="9"/>
     </row>
     <row r="57" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D57" s="332" t="s">
+      <c r="D57" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="E57" s="332"/>
+      <c r="E57" s="342"/>
       <c r="F57" s="131">
         <v>-1524395.48</v>
       </c>
-      <c r="I57" s="333" t="s">
+      <c r="I57" s="343" t="s">
         <v>16</v>
       </c>
-      <c r="J57" s="334"/>
-      <c r="K57" s="335">
+      <c r="J57" s="344"/>
+      <c r="K57" s="345">
         <f>F59+F60+F61</f>
         <v>393764.05999999994</v>
       </c>
-      <c r="L57" s="336"/>
+      <c r="L57" s="346"/>
       <c r="P57" s="36"/>
       <c r="Q57" s="9"/>
     </row>
@@ -9285,11 +9486,11 @@
         <v>18</v>
       </c>
       <c r="J59" s="147"/>
-      <c r="K59" s="337">
+      <c r="K59" s="347">
         <f>-C4</f>
         <v>-373948.72</v>
       </c>
-      <c r="L59" s="338"/>
+      <c r="L59" s="348"/>
     </row>
     <row r="60" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="148" t="s">
@@ -9306,22 +9507,22 @@
       <c r="C61" s="150">
         <v>44955</v>
       </c>
-      <c r="D61" s="339" t="s">
+      <c r="D61" s="349" t="s">
         <v>21</v>
       </c>
-      <c r="E61" s="340"/>
+      <c r="E61" s="350"/>
       <c r="F61" s="151">
         <v>223528.9</v>
       </c>
-      <c r="I61" s="341" t="s">
+      <c r="I61" s="351" t="s">
         <v>22</v>
       </c>
-      <c r="J61" s="342"/>
-      <c r="K61" s="343">
+      <c r="J61" s="352"/>
+      <c r="K61" s="353">
         <f>K57+K59</f>
         <v>19815.339999999967</v>
       </c>
-      <c r="L61" s="343"/>
+      <c r="L61" s="353"/>
     </row>
     <row r="62" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C62" s="152"/>
@@ -10896,23 +11097,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="354"/>
+      <c r="C1" s="356" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="355"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -10925,21 +11126,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="358" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="359"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="360"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="385" t="s">
+      <c r="R3" s="395" t="s">
         <v>2</v>
       </c>
     </row>
@@ -10954,14 +11155,14 @@
       <c r="D4" s="307">
         <v>45081</v>
       </c>
-      <c r="E4" s="355" t="s">
+      <c r="E4" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="356"/>
-      <c r="H4" s="357" t="s">
+      <c r="F4" s="366"/>
+      <c r="H4" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="358"/>
+      <c r="I4" s="368"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -10971,11 +11172,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="371" t="s">
+      <c r="P4" s="381" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="372"/>
-      <c r="R4" s="386"/>
+      <c r="Q4" s="382"/>
+      <c r="R4" s="396"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -12759,11 +12960,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="351">
+      <c r="M45" s="361">
         <f>SUM(M5:M39)</f>
         <v>3170751</v>
       </c>
-      <c r="N45" s="362">
+      <c r="N45" s="372">
         <f>SUM(N5:N39)</f>
         <v>31751.230000000003</v>
       </c>
@@ -12793,8 +12994,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="363"/>
+      <c r="M46" s="362"/>
+      <c r="N46" s="373"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -12886,29 +13087,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="364" t="s">
+      <c r="H51" s="374" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="365"/>
+      <c r="I51" s="375"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="366">
+      <c r="K51" s="376">
         <f>I49+L49</f>
         <v>66093.360000000015</v>
       </c>
-      <c r="L51" s="367"/>
-      <c r="M51" s="368">
+      <c r="L51" s="377"/>
+      <c r="M51" s="378">
         <f>N45+M45</f>
         <v>3202502.23</v>
       </c>
-      <c r="N51" s="369"/>
+      <c r="N51" s="379"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="361" t="s">
+      <c r="D52" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="361"/>
+      <c r="E52" s="371"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>3132761.64</v>
@@ -12919,22 +13120,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="332" t="s">
+      <c r="D53" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="332"/>
+      <c r="E53" s="342"/>
       <c r="F53" s="131">
         <v>-3128572.23</v>
       </c>
-      <c r="I53" s="333" t="s">
+      <c r="I53" s="343" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="334"/>
-      <c r="K53" s="373">
+      <c r="J53" s="344"/>
+      <c r="K53" s="383">
         <f>F55+F56+F57</f>
         <v>417897.52000000014</v>
       </c>
-      <c r="L53" s="374"/>
+      <c r="L53" s="384"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -12965,11 +13166,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="375">
+      <c r="K55" s="385">
         <f>-C4</f>
         <v>-345633.69</v>
       </c>
-      <c r="L55" s="376"/>
+      <c r="L55" s="386"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -12986,22 +13187,22 @@
       <c r="C57" s="150">
         <v>45109</v>
       </c>
-      <c r="D57" s="339" t="s">
+      <c r="D57" s="349" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="340"/>
+      <c r="E57" s="350"/>
       <c r="F57" s="316">
         <v>359108.11</v>
       </c>
-      <c r="I57" s="380" t="s">
+      <c r="I57" s="390" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="381"/>
-      <c r="K57" s="382">
+      <c r="J57" s="391"/>
+      <c r="K57" s="392">
         <f>K53+K55</f>
         <v>72263.830000000133</v>
       </c>
-      <c r="L57" s="382"/>
+      <c r="L57" s="392"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -13162,7 +13363,7 @@
   </sheetPr>
   <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -14533,8 +14734,8 @@
   </sheetPr>
   <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14559,23 +14760,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="354"/>
+      <c r="C1" s="356" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="355"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -14588,21 +14789,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="358" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="359"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="360"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="385" t="s">
+      <c r="R3" s="395" t="s">
         <v>2</v>
       </c>
     </row>
@@ -14617,14 +14818,14 @@
       <c r="D4" s="307">
         <v>45109</v>
       </c>
-      <c r="E4" s="355" t="s">
+      <c r="E4" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="356"/>
-      <c r="H4" s="357" t="s">
+      <c r="F4" s="366"/>
+      <c r="H4" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="358"/>
+      <c r="I4" s="368"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -14634,11 +14835,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="371" t="s">
+      <c r="P4" s="381" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="372"/>
-      <c r="R4" s="386"/>
+      <c r="Q4" s="382"/>
+      <c r="R4" s="396"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -16016,7 +16217,9 @@
     <row r="34" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23"/>
       <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
+      <c r="C34" s="25">
+        <v>854250</v>
+      </c>
       <c r="D34" s="82"/>
       <c r="E34" s="27"/>
       <c r="F34" s="28"/>
@@ -16026,7 +16229,7 @@
       <c r="J34" s="86">
         <v>45111</v>
       </c>
-      <c r="K34" s="387" t="s">
+      <c r="K34" s="332" t="s">
         <v>390</v>
       </c>
       <c r="L34" s="284">
@@ -16041,11 +16244,11 @@
       <c r="O34" s="35"/>
       <c r="P34" s="235">
         <f t="shared" si="0"/>
-        <v>14500</v>
+        <v>868750</v>
       </c>
       <c r="Q34" s="236">
         <f t="shared" si="1"/>
-        <v>14500</v>
+        <v>868750</v>
       </c>
       <c r="R34" s="238">
         <v>0</v>
@@ -16055,7 +16258,9 @@
     <row r="35" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23"/>
       <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
+      <c r="C35" s="25">
+        <v>37120</v>
+      </c>
       <c r="D35" s="77"/>
       <c r="E35" s="27"/>
       <c r="F35" s="28"/>
@@ -16080,11 +16285,11 @@
       <c r="O35" s="35"/>
       <c r="P35" s="235">
         <f t="shared" si="0"/>
-        <v>1392</v>
+        <v>38512</v>
       </c>
       <c r="Q35" s="236">
         <f t="shared" si="1"/>
-        <v>1392</v>
+        <v>38512</v>
       </c>
       <c r="R35" s="238">
         <v>0</v>
@@ -16094,7 +16299,9 @@
     <row r="36" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="23"/>
       <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
+      <c r="C36" s="25">
+        <v>943600</v>
+      </c>
       <c r="D36" s="85"/>
       <c r="E36" s="27"/>
       <c r="F36" s="28"/>
@@ -16119,11 +16326,11 @@
       <c r="O36" s="35"/>
       <c r="P36" s="235">
         <f t="shared" si="0"/>
-        <v>549</v>
+        <v>944149</v>
       </c>
       <c r="Q36" s="236">
         <f t="shared" si="1"/>
-        <v>549</v>
+        <v>944149</v>
       </c>
       <c r="R36" s="238">
         <v>0</v>
@@ -16133,7 +16340,9 @@
     <row r="37" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="23"/>
       <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
+      <c r="C37" s="25">
+        <v>37120</v>
+      </c>
       <c r="D37" s="82"/>
       <c r="E37" s="27"/>
       <c r="F37" s="28"/>
@@ -16412,11 +16621,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="351">
+      <c r="M45" s="361">
         <f>SUM(M5:M39)</f>
         <v>3725440</v>
       </c>
-      <c r="N45" s="362">
+      <c r="N45" s="372">
         <f>SUM(N5:N39)</f>
         <v>22373</v>
       </c>
@@ -16426,7 +16635,7 @@
       </c>
       <c r="Q45" s="236">
         <f>SUM(Q5:Q44)</f>
-        <v>17154</v>
+        <v>1852124</v>
       </c>
       <c r="R45" s="329">
         <f>SUM(R5:R39)</f>
@@ -16446,8 +16655,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="363"/>
+      <c r="M46" s="362"/>
+      <c r="N46" s="373"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="236">
         <f t="shared" si="1"/>
@@ -16503,7 +16712,7 @@
       </c>
       <c r="C49" s="122">
         <f>SUM(C5:C48)</f>
-        <v>83452</v>
+        <v>1955542</v>
       </c>
       <c r="D49" s="123"/>
       <c r="E49" s="124" t="s">
@@ -16545,32 +16754,32 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="364" t="s">
+      <c r="H51" s="374" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="365"/>
+      <c r="I51" s="375"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="366">
+      <c r="K51" s="376">
         <f>I49+L49</f>
         <v>59309.490000000005</v>
       </c>
-      <c r="L51" s="367"/>
-      <c r="M51" s="368">
+      <c r="L51" s="377"/>
+      <c r="M51" s="378">
         <f>N45+M45</f>
         <v>3747813</v>
       </c>
-      <c r="N51" s="369"/>
+      <c r="N51" s="379"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="361" t="s">
+      <c r="D52" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="361"/>
+      <c r="E52" s="371"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
-        <v>3672769.51</v>
+        <v>1800679.5099999998</v>
       </c>
       <c r="I52" s="137"/>
       <c r="J52" s="138"/>
@@ -16578,22 +16787,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="332" t="s">
+      <c r="D53" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="332"/>
+      <c r="E53" s="342"/>
       <c r="F53" s="131">
-        <v>0</v>
-      </c>
-      <c r="I53" s="333" t="s">
+        <v>-2396693.7400000002</v>
+      </c>
+      <c r="I53" s="343" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="334"/>
-      <c r="K53" s="373">
+      <c r="J53" s="344"/>
+      <c r="K53" s="383">
         <f>F55+F56+F57</f>
-        <v>4132439.63</v>
-      </c>
-      <c r="L53" s="374"/>
+        <v>-136344.11000000045</v>
+      </c>
+      <c r="L53" s="384"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -16618,18 +16827,18 @@
       </c>
       <c r="F55" s="131">
         <f>SUM(F52:F54)</f>
-        <v>3672769.51</v>
+        <v>-596014.23000000045</v>
       </c>
       <c r="H55" s="23"/>
       <c r="I55" s="146" t="s">
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="375">
+      <c r="K55" s="385">
         <f>-C4</f>
         <v>-359108.11</v>
       </c>
-      <c r="L55" s="376"/>
+      <c r="L55" s="386"/>
       <c r="Q55" s="9"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -16647,22 +16856,22 @@
       <c r="C57" s="150">
         <v>45137</v>
       </c>
-      <c r="D57" s="339" t="s">
+      <c r="D57" s="349" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="340"/>
+      <c r="E57" s="350"/>
       <c r="F57" s="316">
         <v>358228.12</v>
       </c>
-      <c r="I57" s="380" t="s">
-        <v>22</v>
-      </c>
-      <c r="J57" s="381"/>
-      <c r="K57" s="382">
+      <c r="I57" s="387" t="s">
+        <v>170</v>
+      </c>
+      <c r="J57" s="388"/>
+      <c r="K57" s="397">
         <f>K53+K55</f>
-        <v>3773331.52</v>
-      </c>
-      <c r="L57" s="382"/>
+        <v>-495452.22000000044</v>
+      </c>
+      <c r="L57" s="397"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -16827,12 +17036,13 @@
   <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="206" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="156" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="207" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="209" bestFit="1" customWidth="1"/>
@@ -16844,7 +17054,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="333" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="168"/>
@@ -16856,7 +17066,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="172" t="s">
+      <c r="A2" s="334" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="173" t="s">
@@ -16876,348 +17086,528 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="320"/>
-      <c r="B3" s="321"/>
-      <c r="C3" s="322"/>
+      <c r="A3" s="335">
+        <v>45110</v>
+      </c>
+      <c r="B3" s="341" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3" s="322">
+        <v>127061.9</v>
+      </c>
       <c r="D3" s="244"/>
       <c r="E3" s="220"/>
       <c r="F3" s="180">
         <f>C3-E3</f>
-        <v>0</v>
+        <v>127061.9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="320"/>
-      <c r="B4" s="321"/>
-      <c r="C4" s="322"/>
+      <c r="A4" s="335">
+        <v>45111</v>
+      </c>
+      <c r="B4" s="341" t="s">
+        <v>395</v>
+      </c>
+      <c r="C4" s="322">
+        <v>106089.8</v>
+      </c>
       <c r="D4" s="244"/>
       <c r="E4" s="220"/>
       <c r="F4" s="183">
         <f>C4-E4+F3</f>
-        <v>0</v>
+        <v>233151.7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="320"/>
-      <c r="B5" s="321"/>
-      <c r="C5" s="322"/>
+      <c r="A5" s="335">
+        <v>45112</v>
+      </c>
+      <c r="B5" s="341" t="s">
+        <v>396</v>
+      </c>
+      <c r="C5" s="322">
+        <v>148542.16</v>
+      </c>
       <c r="D5" s="244"/>
       <c r="E5" s="220"/>
       <c r="F5" s="183">
         <f t="shared" ref="F5:F68" si="0">C5-E5+F4</f>
-        <v>0</v>
+        <v>381693.86</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="320"/>
-      <c r="B6" s="321"/>
-      <c r="C6" s="322"/>
+      <c r="A6" s="335">
+        <v>45113</v>
+      </c>
+      <c r="B6" s="341" t="s">
+        <v>397</v>
+      </c>
+      <c r="C6" s="322">
+        <v>91606.01</v>
+      </c>
       <c r="D6" s="244"/>
       <c r="E6" s="220"/>
       <c r="F6" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>473299.87</v>
       </c>
       <c r="G6" s="184"/>
     </row>
     <row r="7" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="320"/>
-      <c r="B7" s="321"/>
-      <c r="C7" s="322"/>
+      <c r="A7" s="335">
+        <v>45114</v>
+      </c>
+      <c r="B7" s="341" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" s="322">
+        <v>139761.34</v>
+      </c>
       <c r="D7" s="244"/>
       <c r="E7" s="220"/>
       <c r="F7" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>613061.21</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="320"/>
-      <c r="B8" s="321"/>
-      <c r="C8" s="322"/>
+      <c r="A8" s="335">
+        <v>45114</v>
+      </c>
+      <c r="B8" s="341" t="s">
+        <v>399</v>
+      </c>
+      <c r="C8" s="322">
+        <v>19507.55</v>
+      </c>
       <c r="D8" s="244"/>
       <c r="E8" s="220"/>
       <c r="F8" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>632568.76</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="320"/>
-      <c r="B9" s="321"/>
-      <c r="C9" s="322"/>
+      <c r="A9" s="335">
+        <v>45115</v>
+      </c>
+      <c r="B9" s="341" t="s">
+        <v>400</v>
+      </c>
+      <c r="C9" s="322">
+        <v>13626</v>
+      </c>
       <c r="D9" s="181"/>
       <c r="E9" s="149"/>
       <c r="F9" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>646194.76</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="320"/>
-      <c r="B10" s="321"/>
-      <c r="C10" s="322"/>
+      <c r="A10" s="335">
+        <v>45115</v>
+      </c>
+      <c r="B10" s="341" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" s="322">
+        <v>137491.6</v>
+      </c>
       <c r="D10" s="181"/>
       <c r="E10" s="149"/>
       <c r="F10" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>783686.36</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="320"/>
-      <c r="B11" s="321"/>
-      <c r="C11" s="322"/>
+      <c r="A11" s="335">
+        <v>45115</v>
+      </c>
+      <c r="B11" s="341" t="s">
+        <v>403</v>
+      </c>
+      <c r="C11" s="322">
+        <v>86570.4</v>
+      </c>
       <c r="D11" s="181"/>
       <c r="E11" s="149"/>
       <c r="F11" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>870256.76</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="320"/>
-      <c r="B12" s="321"/>
-      <c r="C12" s="322"/>
+      <c r="A12" s="335">
+        <v>45117</v>
+      </c>
+      <c r="B12" s="341" t="s">
+        <v>402</v>
+      </c>
+      <c r="C12" s="322">
+        <v>76708.800000000003</v>
+      </c>
       <c r="D12" s="181"/>
       <c r="E12" s="149"/>
       <c r="F12" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>946965.56</v>
       </c>
       <c r="G12" s="184"/>
     </row>
     <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="320"/>
-      <c r="B13" s="321"/>
-      <c r="C13" s="322"/>
+      <c r="A13" s="335">
+        <v>45117</v>
+      </c>
+      <c r="B13" s="341" t="s">
+        <v>404</v>
+      </c>
+      <c r="C13" s="322">
+        <v>47903.7</v>
+      </c>
       <c r="D13" s="181"/>
       <c r="E13" s="149"/>
       <c r="F13" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>994869.26</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="320"/>
-      <c r="B14" s="321"/>
-      <c r="C14" s="322"/>
+      <c r="A14" s="335">
+        <v>45118</v>
+      </c>
+      <c r="B14" s="341" t="s">
+        <v>405</v>
+      </c>
+      <c r="C14" s="322">
+        <v>48347.37</v>
+      </c>
       <c r="D14" s="181"/>
       <c r="E14" s="149"/>
       <c r="F14" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1043216.63</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="320"/>
-      <c r="B15" s="321"/>
-      <c r="C15" s="322"/>
+      <c r="A15" s="335">
+        <v>45118</v>
+      </c>
+      <c r="B15" s="341" t="s">
+        <v>406</v>
+      </c>
+      <c r="C15" s="322">
+        <v>0</v>
+      </c>
       <c r="D15" s="181"/>
       <c r="E15" s="149"/>
       <c r="F15" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1043216.63</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="320"/>
-      <c r="B16" s="321"/>
-      <c r="C16" s="322"/>
+      <c r="A16" s="335">
+        <v>45119</v>
+      </c>
+      <c r="B16" s="341" t="s">
+        <v>407</v>
+      </c>
+      <c r="C16" s="322">
+        <v>0</v>
+      </c>
       <c r="D16" s="181"/>
       <c r="E16" s="149"/>
       <c r="F16" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1043216.63</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="320"/>
-      <c r="B17" s="321"/>
-      <c r="C17" s="322"/>
+      <c r="A17" s="335">
+        <v>45119</v>
+      </c>
+      <c r="B17" s="341" t="s">
+        <v>408</v>
+      </c>
+      <c r="C17" s="322">
+        <v>66833.850000000006</v>
+      </c>
       <c r="D17" s="181"/>
       <c r="E17" s="149"/>
       <c r="F17" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1110050.48</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="320"/>
-      <c r="B18" s="321"/>
-      <c r="C18" s="322"/>
+      <c r="A18" s="335">
+        <v>45119</v>
+      </c>
+      <c r="B18" s="341" t="s">
+        <v>409</v>
+      </c>
+      <c r="C18" s="322">
+        <v>1345.4</v>
+      </c>
       <c r="D18" s="181"/>
       <c r="E18" s="149"/>
       <c r="F18" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1111395.8799999999</v>
       </c>
       <c r="J18" s="133" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="320"/>
-      <c r="B19" s="321"/>
-      <c r="C19" s="322"/>
+      <c r="A19" s="335">
+        <v>45120</v>
+      </c>
+      <c r="B19" s="341" t="s">
+        <v>410</v>
+      </c>
+      <c r="C19" s="322">
+        <v>62164.47</v>
+      </c>
       <c r="D19" s="181"/>
       <c r="E19" s="149"/>
       <c r="F19" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1173560.3499999999</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="320"/>
-      <c r="B20" s="321"/>
-      <c r="C20" s="322"/>
+      <c r="A20" s="335">
+        <v>45121</v>
+      </c>
+      <c r="B20" s="341" t="s">
+        <v>411</v>
+      </c>
+      <c r="C20" s="322">
+        <v>51273.68</v>
+      </c>
       <c r="D20" s="181"/>
       <c r="E20" s="149"/>
       <c r="F20" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1224834.0299999998</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="320"/>
-      <c r="B21" s="321"/>
-      <c r="C21" s="322"/>
+      <c r="A21" s="335">
+        <v>45122</v>
+      </c>
+      <c r="B21" s="341" t="s">
+        <v>412</v>
+      </c>
+      <c r="C21" s="322">
+        <v>0</v>
+      </c>
       <c r="D21" s="181"/>
       <c r="E21" s="149"/>
       <c r="F21" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1224834.0299999998</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="320"/>
-      <c r="B22" s="321"/>
-      <c r="C22" s="322"/>
+      <c r="A22" s="335">
+        <v>45122</v>
+      </c>
+      <c r="B22" s="341" t="s">
+        <v>413</v>
+      </c>
+      <c r="C22" s="322">
+        <v>49319.38</v>
+      </c>
       <c r="D22" s="181"/>
       <c r="E22" s="149"/>
       <c r="F22" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1274153.4099999997</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="320"/>
-      <c r="B23" s="321"/>
-      <c r="C23" s="322"/>
+      <c r="A23" s="335">
+        <v>45122</v>
+      </c>
+      <c r="B23" s="341" t="s">
+        <v>414</v>
+      </c>
+      <c r="C23" s="322">
+        <v>19983.599999999999</v>
+      </c>
       <c r="D23" s="181"/>
       <c r="E23" s="149"/>
       <c r="F23" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1294137.0099999998</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="320"/>
-      <c r="B24" s="321"/>
-      <c r="C24" s="322"/>
+      <c r="A24" s="335">
+        <v>45122</v>
+      </c>
+      <c r="B24" s="341" t="s">
+        <v>415</v>
+      </c>
+      <c r="C24" s="322">
+        <v>60011.519999999997</v>
+      </c>
       <c r="D24" s="181"/>
       <c r="E24" s="149"/>
       <c r="F24" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1354148.5299999998</v>
       </c>
       <c r="G24" s="184"/>
     </row>
     <row r="25" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="320"/>
-      <c r="B25" s="321"/>
-      <c r="C25" s="322"/>
+      <c r="A25" s="335">
+        <v>45124</v>
+      </c>
+      <c r="B25" s="341" t="s">
+        <v>416</v>
+      </c>
+      <c r="C25" s="322">
+        <v>73787.100000000006</v>
+      </c>
       <c r="D25" s="181"/>
       <c r="E25" s="149"/>
       <c r="F25" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1427935.63</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="320"/>
-      <c r="B26" s="321"/>
-      <c r="C26" s="322"/>
+      <c r="A26" s="335">
+        <v>45124</v>
+      </c>
+      <c r="B26" s="341" t="s">
+        <v>417</v>
+      </c>
+      <c r="C26" s="322">
+        <v>81209.850000000006</v>
+      </c>
       <c r="D26" s="181"/>
       <c r="E26" s="149"/>
       <c r="F26" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1509145.48</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="320"/>
-      <c r="B27" s="321"/>
-      <c r="C27" s="322"/>
+      <c r="A27" s="335">
+        <v>45124</v>
+      </c>
+      <c r="B27" s="341" t="s">
+        <v>418</v>
+      </c>
+      <c r="C27" s="322">
+        <v>0</v>
+      </c>
       <c r="D27" s="181"/>
       <c r="E27" s="149"/>
       <c r="F27" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1509145.48</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="320"/>
-      <c r="B28" s="321"/>
-      <c r="C28" s="322"/>
+      <c r="A28" s="335">
+        <v>45125</v>
+      </c>
+      <c r="B28" s="341" t="s">
+        <v>419</v>
+      </c>
+      <c r="C28" s="322">
+        <v>16014</v>
+      </c>
       <c r="D28" s="181"/>
       <c r="E28" s="149"/>
       <c r="F28" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1525159.48</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="320"/>
-      <c r="B29" s="321"/>
-      <c r="C29" s="322"/>
+      <c r="A29" s="335">
+        <v>45125</v>
+      </c>
+      <c r="B29" s="341" t="s">
+        <v>420</v>
+      </c>
+      <c r="C29" s="322">
+        <v>0</v>
+      </c>
       <c r="D29" s="181"/>
       <c r="E29" s="149"/>
       <c r="F29" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1525159.48</v>
       </c>
       <c r="J29" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="320"/>
-      <c r="B30" s="321"/>
-      <c r="C30" s="322"/>
+      <c r="A30" s="335">
+        <v>45125</v>
+      </c>
+      <c r="B30" s="341" t="s">
+        <v>421</v>
+      </c>
+      <c r="C30" s="322">
+        <v>17158</v>
+      </c>
       <c r="D30" s="181"/>
       <c r="E30" s="149"/>
       <c r="F30" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1542317.48</v>
       </c>
       <c r="J30" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="320"/>
-      <c r="B31" s="321"/>
-      <c r="C31" s="322"/>
+      <c r="A31" s="335">
+        <v>45125</v>
+      </c>
+      <c r="B31" s="341" t="s">
+        <v>422</v>
+      </c>
+      <c r="C31" s="322">
+        <v>39357.599999999999</v>
+      </c>
       <c r="D31" s="181"/>
       <c r="E31" s="149"/>
       <c r="F31" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1581675.08</v>
       </c>
       <c r="J31" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="320"/>
-      <c r="B32" s="321"/>
-      <c r="C32" s="322"/>
+      <c r="A32" s="335">
+        <v>45126</v>
+      </c>
+      <c r="B32" s="341" t="s">
+        <v>423</v>
+      </c>
+      <c r="C32" s="322">
+        <v>79733.740000000005</v>
+      </c>
       <c r="D32" s="181"/>
       <c r="E32" s="149"/>
       <c r="F32" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1661408.82</v>
       </c>
       <c r="G32" s="184"/>
       <c r="J32" s="149">
@@ -17225,70 +17615,100 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="320"/>
-      <c r="B33" s="321"/>
-      <c r="C33" s="322"/>
+      <c r="A33" s="335">
+        <v>45126</v>
+      </c>
+      <c r="B33" s="341" t="s">
+        <v>424</v>
+      </c>
+      <c r="C33" s="322">
+        <v>0</v>
+      </c>
       <c r="D33" s="181"/>
       <c r="E33" s="149"/>
       <c r="F33" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1661408.82</v>
       </c>
       <c r="J33" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="320"/>
-      <c r="B34" s="321"/>
-      <c r="C34" s="322"/>
+      <c r="A34" s="335">
+        <v>45126</v>
+      </c>
+      <c r="B34" s="341" t="s">
+        <v>425</v>
+      </c>
+      <c r="C34" s="322">
+        <v>594</v>
+      </c>
       <c r="D34" s="181"/>
       <c r="E34" s="149"/>
       <c r="F34" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1662002.82</v>
       </c>
       <c r="J34" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="320"/>
-      <c r="B35" s="321"/>
-      <c r="C35" s="322"/>
+      <c r="A35" s="335">
+        <v>45126</v>
+      </c>
+      <c r="B35" s="341" t="s">
+        <v>426</v>
+      </c>
+      <c r="C35" s="322">
+        <v>0</v>
+      </c>
       <c r="D35" s="181"/>
       <c r="E35" s="149"/>
       <c r="F35" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1662002.82</v>
       </c>
       <c r="J35" s="149">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="320"/>
-      <c r="B36" s="321"/>
-      <c r="C36" s="322"/>
+      <c r="A36" s="335">
+        <v>45127</v>
+      </c>
+      <c r="B36" s="341" t="s">
+        <v>427</v>
+      </c>
+      <c r="C36" s="322">
+        <v>0</v>
+      </c>
       <c r="D36" s="181"/>
       <c r="E36" s="149"/>
       <c r="F36" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1662002.82</v>
       </c>
       <c r="J36" s="133">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="320"/>
-      <c r="B37" s="321"/>
-      <c r="C37" s="322"/>
+      <c r="A37" s="335">
+        <v>45127</v>
+      </c>
+      <c r="B37" s="341" t="s">
+        <v>428</v>
+      </c>
+      <c r="C37" s="322">
+        <v>89753.15</v>
+      </c>
       <c r="D37" s="181"/>
       <c r="E37" s="149"/>
       <c r="F37" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1751755.97</v>
       </c>
       <c r="J37" s="187">
         <f>SUM(J29:J36)</f>
@@ -17296,447 +17716,579 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="320"/>
-      <c r="B38" s="321"/>
-      <c r="C38" s="322"/>
+      <c r="A38" s="335">
+        <v>45128</v>
+      </c>
+      <c r="B38" s="341" t="s">
+        <v>429</v>
+      </c>
+      <c r="C38" s="322">
+        <v>8469.0499999999993</v>
+      </c>
       <c r="D38" s="181"/>
       <c r="E38" s="149"/>
       <c r="F38" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1760225.02</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="320"/>
-      <c r="B39" s="321"/>
-      <c r="C39" s="322"/>
+      <c r="A39" s="335">
+        <v>45128</v>
+      </c>
+      <c r="B39" s="341" t="s">
+        <v>430</v>
+      </c>
+      <c r="C39" s="322">
+        <v>69894.600000000006</v>
+      </c>
       <c r="D39" s="181"/>
       <c r="E39" s="149"/>
       <c r="F39" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1830119.62</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="320"/>
-      <c r="B40" s="321"/>
-      <c r="C40" s="322"/>
+      <c r="A40" s="335">
+        <v>45128</v>
+      </c>
+      <c r="B40" s="341" t="s">
+        <v>431</v>
+      </c>
+      <c r="C40" s="322">
+        <v>0</v>
+      </c>
       <c r="D40" s="181"/>
       <c r="E40" s="100"/>
       <c r="F40" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1830119.62</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="320"/>
-      <c r="B41" s="321"/>
-      <c r="C41" s="322"/>
+      <c r="A41" s="335">
+        <v>45128</v>
+      </c>
+      <c r="B41" s="341" t="s">
+        <v>432</v>
+      </c>
+      <c r="C41" s="322">
+        <v>3432.8</v>
+      </c>
       <c r="D41" s="181"/>
       <c r="E41" s="100"/>
       <c r="F41" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1833552.4200000002</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="320"/>
-      <c r="B42" s="321"/>
-      <c r="C42" s="322"/>
+      <c r="A42" s="335">
+        <v>45128</v>
+      </c>
+      <c r="B42" s="341" t="s">
+        <v>433</v>
+      </c>
+      <c r="C42" s="322">
+        <v>0</v>
+      </c>
       <c r="D42" s="185"/>
       <c r="E42" s="100"/>
       <c r="F42" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1833552.4200000002</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="320"/>
-      <c r="B43" s="321"/>
-      <c r="C43" s="322"/>
+      <c r="A43" s="335">
+        <v>45129</v>
+      </c>
+      <c r="B43" s="341" t="s">
+        <v>434</v>
+      </c>
+      <c r="C43" s="322">
+        <v>0</v>
+      </c>
       <c r="D43" s="192"/>
       <c r="E43" s="100"/>
       <c r="F43" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1833552.4200000002</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="320"/>
-      <c r="B44" s="321"/>
-      <c r="C44" s="322"/>
+      <c r="A44" s="335">
+        <v>45129</v>
+      </c>
+      <c r="B44" s="341" t="s">
+        <v>435</v>
+      </c>
+      <c r="C44" s="322">
+        <v>55115.4</v>
+      </c>
       <c r="D44" s="192"/>
       <c r="E44" s="100"/>
       <c r="F44" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1888667.82</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="320"/>
-      <c r="B45" s="321"/>
-      <c r="C45" s="322"/>
+      <c r="A45" s="335">
+        <v>45129</v>
+      </c>
+      <c r="B45" s="341" t="s">
+        <v>436</v>
+      </c>
+      <c r="C45" s="322">
+        <v>66157.350000000006</v>
+      </c>
       <c r="D45" s="192"/>
       <c r="E45" s="100"/>
       <c r="F45" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1954825.1700000002</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="320"/>
-      <c r="B46" s="321"/>
-      <c r="C46" s="322"/>
+      <c r="A46" s="335">
+        <v>45129</v>
+      </c>
+      <c r="B46" s="341" t="s">
+        <v>437</v>
+      </c>
+      <c r="C46" s="322">
+        <v>1730.4</v>
+      </c>
       <c r="D46" s="192"/>
       <c r="E46" s="100"/>
       <c r="F46" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1956555.57</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="325"/>
-      <c r="B47" s="321"/>
-      <c r="C47" s="322"/>
+      <c r="A47" s="335">
+        <v>45131</v>
+      </c>
+      <c r="B47" s="341" t="s">
+        <v>438</v>
+      </c>
+      <c r="C47" s="322">
+        <v>8367.4</v>
+      </c>
       <c r="D47" s="192"/>
       <c r="E47" s="100"/>
       <c r="F47" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1964922.97</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="325"/>
-      <c r="B48" s="321"/>
-      <c r="C48" s="322"/>
+      <c r="A48" s="335">
+        <v>45131</v>
+      </c>
+      <c r="B48" s="341" t="s">
+        <v>439</v>
+      </c>
+      <c r="C48" s="322">
+        <v>69725.83</v>
+      </c>
       <c r="D48" s="192"/>
       <c r="E48" s="100"/>
       <c r="F48" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2034648.8</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="325"/>
-      <c r="B49" s="321"/>
-      <c r="C49" s="322"/>
+      <c r="A49" s="335">
+        <v>45133</v>
+      </c>
+      <c r="B49" s="341" t="s">
+        <v>440</v>
+      </c>
+      <c r="C49" s="322">
+        <v>71238.23</v>
+      </c>
       <c r="D49" s="192"/>
       <c r="E49" s="100"/>
       <c r="F49" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2105887.0300000003</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="325"/>
-      <c r="B50" s="321"/>
-      <c r="C50" s="322"/>
+      <c r="A50" s="335">
+        <v>45133</v>
+      </c>
+      <c r="B50" s="341" t="s">
+        <v>441</v>
+      </c>
+      <c r="C50" s="322">
+        <v>0</v>
+      </c>
       <c r="D50" s="192"/>
       <c r="E50" s="100"/>
       <c r="F50" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2105887.0300000003</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="325"/>
-      <c r="B51" s="321"/>
-      <c r="C51" s="322"/>
+      <c r="A51" s="335">
+        <v>45134</v>
+      </c>
+      <c r="B51" s="341" t="s">
+        <v>442</v>
+      </c>
+      <c r="C51" s="322">
+        <v>0</v>
+      </c>
       <c r="D51" s="192"/>
       <c r="E51" s="100"/>
       <c r="F51" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2105887.0300000003</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="324"/>
-      <c r="B52" s="248"/>
-      <c r="C52" s="149"/>
+      <c r="A52" s="336">
+        <v>45134</v>
+      </c>
+      <c r="B52" s="248" t="s">
+        <v>443</v>
+      </c>
+      <c r="C52" s="149">
+        <v>68136.3</v>
+      </c>
       <c r="D52" s="192"/>
       <c r="E52" s="100"/>
       <c r="F52" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2174023.33</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="324"/>
-      <c r="B53" s="248"/>
-      <c r="C53" s="149"/>
+      <c r="A53" s="336">
+        <v>45135</v>
+      </c>
+      <c r="B53" s="248" t="s">
+        <v>444</v>
+      </c>
+      <c r="C53" s="149">
+        <v>331.8</v>
+      </c>
       <c r="D53" s="192"/>
       <c r="E53" s="100"/>
       <c r="F53" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2174355.13</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="324"/>
-      <c r="B54" s="248"/>
-      <c r="C54" s="149"/>
+      <c r="A54" s="336">
+        <v>45135</v>
+      </c>
+      <c r="B54" s="248" t="s">
+        <v>445</v>
+      </c>
+      <c r="C54" s="149">
+        <v>79638.87</v>
+      </c>
       <c r="D54" s="192"/>
       <c r="E54" s="100"/>
       <c r="F54" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2253994</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="246"/>
-      <c r="B55" s="248"/>
-      <c r="C55" s="149"/>
+      <c r="A55" s="336">
+        <v>45135</v>
+      </c>
+      <c r="B55" s="248" t="s">
+        <v>446</v>
+      </c>
+      <c r="C55" s="149">
+        <v>0</v>
+      </c>
       <c r="D55" s="192"/>
       <c r="E55" s="100"/>
       <c r="F55" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2253994</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="246"/>
-      <c r="B56" s="248"/>
-      <c r="C56" s="149"/>
+      <c r="A56" s="336">
+        <v>45135</v>
+      </c>
+      <c r="B56" s="248" t="s">
+        <v>447</v>
+      </c>
+      <c r="C56" s="149">
+        <v>27350.46</v>
+      </c>
       <c r="D56" s="192"/>
       <c r="E56" s="100"/>
       <c r="F56" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="193"/>
-      <c r="B57" s="194"/>
-      <c r="C57" s="100"/>
+        <v>2281344.46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="337">
+        <v>45136</v>
+      </c>
+      <c r="B57" s="194" t="s">
+        <v>448</v>
+      </c>
+      <c r="C57" s="100">
+        <v>0</v>
+      </c>
       <c r="D57" s="192"/>
       <c r="E57" s="100"/>
       <c r="F57" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="193"/>
-      <c r="B58" s="194"/>
-      <c r="C58" s="100"/>
+        <v>2281344.46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="337">
+        <v>45136</v>
+      </c>
+      <c r="B58" s="194" t="s">
+        <v>449</v>
+      </c>
+      <c r="C58" s="100">
+        <v>60701.279999999999</v>
+      </c>
       <c r="D58" s="192"/>
       <c r="E58" s="100"/>
       <c r="F58" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="193"/>
-      <c r="B59" s="194"/>
-      <c r="C59" s="100"/>
+        <v>2342045.7399999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="337">
+        <v>45136</v>
+      </c>
+      <c r="B59" s="194" t="s">
+        <v>450</v>
+      </c>
+      <c r="C59" s="100">
+        <v>54648</v>
+      </c>
       <c r="D59" s="192"/>
       <c r="E59" s="100"/>
       <c r="F59" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="193"/>
+        <v>2396693.7399999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="337"/>
       <c r="B60" s="194"/>
       <c r="C60" s="100"/>
       <c r="D60" s="192"/>
       <c r="E60" s="100"/>
       <c r="F60" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="193"/>
+        <v>2396693.7399999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="337"/>
       <c r="B61" s="194"/>
       <c r="C61" s="100"/>
       <c r="D61" s="192"/>
       <c r="E61" s="100"/>
       <c r="F61" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="195"/>
+        <v>2396693.7399999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="338"/>
       <c r="B62" s="196"/>
       <c r="C62" s="36"/>
       <c r="D62" s="197"/>
       <c r="E62" s="36"/>
       <c r="F62" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="195"/>
+      <c r="A63" s="338"/>
       <c r="B63" s="196"/>
       <c r="C63" s="36"/>
       <c r="D63" s="197"/>
       <c r="E63" s="36"/>
       <c r="F63" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="195"/>
+      <c r="A64" s="338"/>
       <c r="B64" s="196"/>
       <c r="C64" s="36"/>
       <c r="D64" s="197"/>
       <c r="E64" s="36"/>
       <c r="F64" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="195"/>
+      <c r="A65" s="338"/>
       <c r="B65" s="196"/>
       <c r="C65" s="36"/>
       <c r="D65" s="197"/>
       <c r="E65" s="36"/>
       <c r="F65" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="195"/>
+      <c r="A66" s="338"/>
       <c r="B66" s="196"/>
       <c r="C66" s="36"/>
       <c r="D66" s="197"/>
       <c r="E66" s="36"/>
       <c r="F66" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="195"/>
+      <c r="A67" s="338"/>
       <c r="B67" s="196"/>
       <c r="C67" s="36"/>
       <c r="D67" s="197"/>
       <c r="E67" s="36"/>
       <c r="F67" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="193"/>
+      <c r="A68" s="337"/>
       <c r="B68" s="198"/>
       <c r="C68" s="100"/>
       <c r="D68" s="192"/>
       <c r="E68" s="100"/>
       <c r="F68" s="183">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="193"/>
+      <c r="A69" s="337"/>
       <c r="B69" s="198"/>
       <c r="C69" s="100"/>
       <c r="D69" s="192"/>
       <c r="E69" s="100"/>
       <c r="F69" s="183">
         <f t="shared" ref="F69:F78" si="1">C69-E69+F68</f>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="193"/>
+      <c r="A70" s="337"/>
       <c r="B70" s="198"/>
       <c r="C70" s="100"/>
       <c r="D70" s="192"/>
       <c r="E70" s="100"/>
       <c r="F70" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="193"/>
+      <c r="A71" s="337"/>
       <c r="B71" s="198"/>
       <c r="C71" s="100"/>
       <c r="D71" s="192"/>
       <c r="E71" s="100"/>
       <c r="F71" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="193"/>
+      <c r="A72" s="337"/>
       <c r="B72" s="198"/>
       <c r="C72" s="100"/>
       <c r="D72" s="192"/>
       <c r="E72" s="100"/>
       <c r="F72" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="193"/>
+      <c r="A73" s="337"/>
       <c r="B73" s="198"/>
       <c r="C73" s="100"/>
       <c r="D73" s="192"/>
       <c r="E73" s="100"/>
       <c r="F73" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="193"/>
+      <c r="A74" s="337"/>
       <c r="B74" s="198"/>
       <c r="C74" s="100"/>
       <c r="D74" s="192"/>
       <c r="E74" s="100"/>
       <c r="F74" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="193"/>
+      <c r="A75" s="337"/>
       <c r="B75" s="198"/>
       <c r="C75" s="100"/>
       <c r="D75" s="192"/>
       <c r="E75" s="100"/>
       <c r="F75" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="193"/>
+      <c r="A76" s="337"/>
       <c r="B76" s="198"/>
       <c r="C76" s="100"/>
       <c r="D76" s="192"/>
       <c r="E76" s="100"/>
       <c r="F76" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="193"/>
+      <c r="A77" s="337"/>
       <c r="B77" s="198"/>
       <c r="C77" s="100"/>
       <c r="D77" s="192"/>
       <c r="E77" s="100"/>
       <c r="F77" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="199"/>
+      <c r="A78" s="339"/>
       <c r="B78" s="200"/>
       <c r="C78" s="36">
         <v>0</v>
@@ -17745,15 +18297,15 @@
       <c r="E78" s="36"/>
       <c r="F78" s="183">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="201"/>
+      <c r="A79" s="340"/>
       <c r="B79" s="202"/>
       <c r="C79" s="317">
         <f>SUM(C3:C78)</f>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
       <c r="D79" s="175"/>
       <c r="E79" s="204">
@@ -17762,7 +18314,7 @@
       </c>
       <c r="F79" s="205">
         <f>F78</f>
-        <v>0</v>
+        <v>2396693.7399999998</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -17905,6 +18457,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19279,23 +19832,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="354"/>
+      <c r="C1" s="356" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="355"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -19305,21 +19858,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="358" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="359"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="360"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="353" t="s">
+      <c r="R3" s="363" t="s">
         <v>2</v>
       </c>
     </row>
@@ -19334,14 +19887,14 @@
       <c r="D4" s="17">
         <v>44955</v>
       </c>
-      <c r="E4" s="355" t="s">
+      <c r="E4" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="356"/>
-      <c r="H4" s="357" t="s">
+      <c r="F4" s="366"/>
+      <c r="H4" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="358"/>
+      <c r="I4" s="368"/>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
@@ -19351,11 +19904,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="371" t="s">
+      <c r="P4" s="381" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="372"/>
-      <c r="R4" s="370"/>
+      <c r="Q4" s="382"/>
+      <c r="R4" s="380"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -21156,11 +21709,11 @@
       <c r="J45" s="74"/>
       <c r="K45" s="97"/>
       <c r="L45" s="76"/>
-      <c r="M45" s="351">
+      <c r="M45" s="361">
         <f>SUM(M5:M39)</f>
         <v>2238523</v>
       </c>
-      <c r="N45" s="362">
+      <c r="N45" s="372">
         <f>SUM(N5:N39)</f>
         <v>97258</v>
       </c>
@@ -21190,8 +21743,8 @@
       <c r="J46" s="74"/>
       <c r="K46" s="102"/>
       <c r="L46" s="76"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="363"/>
+      <c r="M46" s="362"/>
+      <c r="N46" s="373"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -21283,29 +21836,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="364" t="s">
+      <c r="H51" s="374" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="365"/>
+      <c r="I51" s="375"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="366">
+      <c r="K51" s="376">
         <f>I49+L49</f>
         <v>90767.040000000008</v>
       </c>
-      <c r="L51" s="367"/>
-      <c r="M51" s="368">
+      <c r="L51" s="377"/>
+      <c r="M51" s="378">
         <f>N45+M45</f>
         <v>2335781</v>
       </c>
-      <c r="N51" s="369"/>
+      <c r="N51" s="379"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D52" s="361" t="s">
+      <c r="D52" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="361"/>
+      <c r="E52" s="371"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2261973.96</v>
@@ -21316,22 +21869,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D53" s="332" t="s">
+      <c r="D53" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="332"/>
+      <c r="E53" s="342"/>
       <c r="F53" s="131">
         <v>-2224189.7400000002</v>
       </c>
-      <c r="I53" s="333" t="s">
+      <c r="I53" s="343" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="334"/>
-      <c r="K53" s="335">
+      <c r="J53" s="344"/>
+      <c r="K53" s="345">
         <f>F55+F56+F57</f>
         <v>296963.76999999973</v>
       </c>
-      <c r="L53" s="336"/>
+      <c r="L53" s="346"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -21362,11 +21915,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="337">
+      <c r="K55" s="347">
         <f>-C4</f>
         <v>-223528.9</v>
       </c>
-      <c r="L55" s="338"/>
+      <c r="L55" s="348"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -21383,22 +21936,22 @@
       <c r="C57" s="150">
         <v>44985</v>
       </c>
-      <c r="D57" s="339" t="s">
+      <c r="D57" s="349" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="340"/>
+      <c r="E57" s="350"/>
       <c r="F57" s="151">
         <v>230554.55</v>
       </c>
-      <c r="I57" s="341" t="s">
+      <c r="I57" s="351" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="342"/>
-      <c r="K57" s="343">
+      <c r="J57" s="352"/>
+      <c r="K57" s="353">
         <f>K53+K55</f>
         <v>73434.869999999733</v>
       </c>
-      <c r="L57" s="343"/>
+      <c r="L57" s="353"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -23002,23 +23555,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="354"/>
+      <c r="C1" s="356" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="355"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -23028,21 +23581,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="358" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="359"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="360"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="353" t="s">
+      <c r="R3" s="363" t="s">
         <v>2</v>
       </c>
     </row>
@@ -23057,14 +23610,14 @@
       <c r="D4" s="17">
         <v>44985</v>
       </c>
-      <c r="E4" s="355" t="s">
+      <c r="E4" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="356"/>
-      <c r="H4" s="357" t="s">
+      <c r="F4" s="366"/>
+      <c r="H4" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="358"/>
+      <c r="I4" s="368"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -23074,11 +23627,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="371" t="s">
+      <c r="P4" s="381" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="372"/>
-      <c r="R4" s="370"/>
+      <c r="Q4" s="382"/>
+      <c r="R4" s="380"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -24871,11 +25424,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="231"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="351">
+      <c r="M45" s="361">
         <f>SUM(M5:M39)</f>
         <v>2689952</v>
       </c>
-      <c r="N45" s="362">
+      <c r="N45" s="372">
         <f>SUM(N5:N39)</f>
         <v>61422</v>
       </c>
@@ -24905,8 +25458,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="363"/>
+      <c r="M46" s="362"/>
+      <c r="N46" s="373"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -24998,29 +25551,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="364" t="s">
+      <c r="H51" s="374" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="365"/>
+      <c r="I51" s="375"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="366">
+      <c r="K51" s="376">
         <f>I49+L49</f>
         <v>425400.67</v>
       </c>
-      <c r="L51" s="367"/>
-      <c r="M51" s="368">
+      <c r="L51" s="377"/>
+      <c r="M51" s="378">
         <f>N45+M45</f>
         <v>2751374</v>
       </c>
-      <c r="N51" s="369"/>
+      <c r="N51" s="379"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="361" t="s">
+      <c r="D52" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="361"/>
+      <c r="E52" s="371"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2464124.33</v>
@@ -25031,22 +25584,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="332" t="s">
+      <c r="D53" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="332"/>
+      <c r="E53" s="342"/>
       <c r="F53" s="131">
         <v>-2869426.04</v>
       </c>
-      <c r="I53" s="333" t="s">
+      <c r="I53" s="343" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="334"/>
-      <c r="K53" s="373">
+      <c r="J53" s="344"/>
+      <c r="K53" s="383">
         <f>F55+F56+F57</f>
         <v>-32021.369999999937</v>
       </c>
-      <c r="L53" s="374"/>
+      <c r="L53" s="384"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -25077,11 +25630,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="375">
+      <c r="K55" s="385">
         <f>-C4</f>
         <v>-230554.55</v>
       </c>
-      <c r="L55" s="376"/>
+      <c r="L55" s="386"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -25098,22 +25651,22 @@
       <c r="C57" s="150">
         <v>45015</v>
       </c>
-      <c r="D57" s="339" t="s">
+      <c r="D57" s="349" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="340"/>
+      <c r="E57" s="350"/>
       <c r="F57" s="151">
         <v>341192.34</v>
       </c>
-      <c r="I57" s="377" t="s">
+      <c r="I57" s="387" t="s">
         <v>170</v>
       </c>
-      <c r="J57" s="378"/>
-      <c r="K57" s="379">
+      <c r="J57" s="388"/>
+      <c r="K57" s="389">
         <f>K53+K55</f>
         <v>-262575.91999999993</v>
       </c>
-      <c r="L57" s="379"/>
+      <c r="L57" s="389"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -26660,23 +27213,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="354"/>
+      <c r="C1" s="356" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="355"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -26689,21 +27242,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="358" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="359"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="360"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="383" t="s">
+      <c r="R3" s="393" t="s">
         <v>2</v>
       </c>
     </row>
@@ -26718,14 +27271,14 @@
       <c r="D4" s="17">
         <v>45015</v>
       </c>
-      <c r="E4" s="355" t="s">
+      <c r="E4" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="356"/>
-      <c r="H4" s="357" t="s">
+      <c r="F4" s="366"/>
+      <c r="H4" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="358"/>
+      <c r="I4" s="368"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -26735,11 +27288,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="371" t="s">
+      <c r="P4" s="381" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="372"/>
-      <c r="R4" s="384"/>
+      <c r="Q4" s="382"/>
+      <c r="R4" s="394"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -28626,11 +29179,11 @@
       <c r="L45" s="312">
         <v>2123.98</v>
       </c>
-      <c r="M45" s="351">
+      <c r="M45" s="361">
         <f>SUM(M5:M39)</f>
         <v>2488709</v>
       </c>
-      <c r="N45" s="362">
+      <c r="N45" s="372">
         <f>SUM(N5:N39)</f>
         <v>78710</v>
       </c>
@@ -28666,8 +29219,8 @@
       <c r="L46" s="281">
         <v>34015</v>
       </c>
-      <c r="M46" s="352"/>
-      <c r="N46" s="363"/>
+      <c r="M46" s="362"/>
+      <c r="N46" s="373"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -28759,29 +29312,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="364" t="s">
+      <c r="H51" s="374" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="365"/>
+      <c r="I51" s="375"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="366">
+      <c r="K51" s="376">
         <f>I49+L49</f>
         <v>124244.06999999999</v>
       </c>
-      <c r="L51" s="367"/>
-      <c r="M51" s="368">
+      <c r="L51" s="377"/>
+      <c r="M51" s="378">
         <f>N45+M45</f>
         <v>2567419</v>
       </c>
-      <c r="N51" s="369"/>
+      <c r="N51" s="379"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="361" t="s">
+      <c r="D52" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="361"/>
+      <c r="E52" s="371"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2480239.9300000002</v>
@@ -28792,22 +29345,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="332" t="s">
+      <c r="D53" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="332"/>
+      <c r="E53" s="342"/>
       <c r="F53" s="131">
         <v>-2463938.5299999998</v>
       </c>
-      <c r="I53" s="333" t="s">
+      <c r="I53" s="343" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="334"/>
-      <c r="K53" s="373">
+      <c r="J53" s="344"/>
+      <c r="K53" s="383">
         <f>F55+F56+F57</f>
         <v>439109.10000000038</v>
       </c>
-      <c r="L53" s="374"/>
+      <c r="L53" s="384"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -28838,11 +29391,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="375">
+      <c r="K55" s="385">
         <f>-C4</f>
         <v>-341192.34</v>
       </c>
-      <c r="L55" s="376"/>
+      <c r="L55" s="386"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -28859,22 +29412,22 @@
       <c r="C57" s="150">
         <v>45050</v>
       </c>
-      <c r="D57" s="339" t="s">
+      <c r="D57" s="349" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="340"/>
+      <c r="E57" s="350"/>
       <c r="F57" s="151">
         <v>394548.7</v>
       </c>
-      <c r="I57" s="380" t="s">
+      <c r="I57" s="390" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="381"/>
-      <c r="K57" s="382">
+      <c r="J57" s="391"/>
+      <c r="K57" s="392">
         <f>K53+K55</f>
         <v>97916.760000000359</v>
       </c>
-      <c r="L57" s="382"/>
+      <c r="L57" s="392"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -30411,23 +30964,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="354"/>
+      <c r="C1" s="356" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="355"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -30440,21 +30993,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="358" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="359"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="360"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="385" t="s">
+      <c r="R3" s="395" t="s">
         <v>2</v>
       </c>
     </row>
@@ -30469,14 +31022,14 @@
       <c r="D4" s="307">
         <v>45050</v>
       </c>
-      <c r="E4" s="355" t="s">
+      <c r="E4" s="365" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="356"/>
-      <c r="H4" s="357" t="s">
+      <c r="F4" s="366"/>
+      <c r="H4" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="358"/>
+      <c r="I4" s="368"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -30486,11 +31039,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="371" t="s">
+      <c r="P4" s="381" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="372"/>
-      <c r="R4" s="386"/>
+      <c r="Q4" s="382"/>
+      <c r="R4" s="396"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -32363,11 +32916,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="351">
+      <c r="M45" s="361">
         <f>SUM(M5:M39)</f>
         <v>3007589</v>
       </c>
-      <c r="N45" s="362">
+      <c r="N45" s="372">
         <f>SUM(N5:N39)</f>
         <v>29752</v>
       </c>
@@ -32397,8 +32950,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="363"/>
+      <c r="M46" s="362"/>
+      <c r="N46" s="373"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -32490,29 +33043,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="364" t="s">
+      <c r="H51" s="374" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="365"/>
+      <c r="I51" s="375"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="366">
+      <c r="K51" s="376">
         <f>I49+L49</f>
         <v>84500.43</v>
       </c>
-      <c r="L51" s="367"/>
-      <c r="M51" s="368">
+      <c r="L51" s="377"/>
+      <c r="M51" s="378">
         <f>N45+M45</f>
         <v>3037341</v>
       </c>
-      <c r="N51" s="369"/>
+      <c r="N51" s="379"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="361" t="s">
+      <c r="D52" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="361"/>
+      <c r="E52" s="371"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2988109.57</v>
@@ -32523,22 +33076,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="332" t="s">
+      <c r="D53" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="332"/>
+      <c r="E53" s="342"/>
       <c r="F53" s="131">
         <v>-2955802.29</v>
       </c>
-      <c r="I53" s="333" t="s">
+      <c r="I53" s="343" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="334"/>
-      <c r="K53" s="373">
+      <c r="J53" s="344"/>
+      <c r="K53" s="383">
         <f>F55+F56+F57</f>
         <v>419364.9699999998</v>
       </c>
-      <c r="L53" s="374"/>
+      <c r="L53" s="384"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -32569,11 +33122,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="375">
+      <c r="K55" s="385">
         <f>-C4</f>
         <v>-394548.7</v>
       </c>
-      <c r="L55" s="376"/>
+      <c r="L55" s="386"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -32590,22 +33143,22 @@
       <c r="C57" s="150">
         <v>45081</v>
       </c>
-      <c r="D57" s="339" t="s">
+      <c r="D57" s="349" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="340"/>
+      <c r="E57" s="350"/>
       <c r="F57" s="316">
         <v>345633.69</v>
       </c>
-      <c r="I57" s="380" t="s">
+      <c r="I57" s="390" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="381"/>
-      <c r="K57" s="382">
+      <c r="J57" s="391"/>
+      <c r="K57" s="392">
         <f>K53+K55</f>
         <v>24816.269999999786</v>
       </c>
-      <c r="L57" s="382"/>
+      <c r="L57" s="392"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>

</xml_diff>